<commit_message>
Rapport de Ndeye Mareme NDIAYE
</commit_message>
<xml_diff>
--- a/Donnees_RZ.xlsx
+++ b/Donnees_RZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479FB5D7-EDAB-4C3B-97BB-638DD05E4359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13915340-163A-4D7B-96D8-DD8B3FF5D32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="213">
   <si>
     <t>Date</t>
   </si>
@@ -630,6 +630,48 @@
   </si>
   <si>
     <t>Livraison le 02septembre</t>
+  </si>
+  <si>
+    <t>Ndeury Touré</t>
+  </si>
+  <si>
+    <t>Elhadji Niang</t>
+  </si>
+  <si>
+    <t>Mandalé Diawné</t>
+  </si>
+  <si>
+    <t>Serigne Fall</t>
+  </si>
+  <si>
+    <t>Beye &amp; frères</t>
+  </si>
+  <si>
+    <t>Tidiane Ba</t>
+  </si>
+  <si>
+    <t>Malick</t>
+  </si>
+  <si>
+    <t>Bassirou Diaw</t>
+  </si>
+  <si>
+    <t>Grand Yoff</t>
+  </si>
+  <si>
+    <t>Dame DIOP</t>
+  </si>
+  <si>
+    <t>Commande livre Aujourd'hui</t>
+  </si>
+  <si>
+    <t>Youssoupha Kane</t>
+  </si>
+  <si>
+    <t>Il connaît non produit</t>
+  </si>
+  <si>
+    <t>Moussa Sall</t>
   </si>
 </sst>
 </file>
@@ -693,7 +735,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -718,6 +760,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,10 +776,10 @@
   <dxfs count="17">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -885,8 +936,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P89" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14">
-  <autoFilter ref="A1:P89" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P102" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14">
+  <autoFilter ref="A1:P102" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{F85C405C-E78B-4DA6-8568-08107D7551E4}" name="Date" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{24A95AD6-D6B8-4864-9451-50BFB3565C62}" name="Prenom_Nom_RZ"/>
@@ -902,10 +953,10 @@
     <tableColumn id="14" xr3:uid="{8DD706C4-BCF7-47C0-9913-F482F7A2F321}" name="Quantites" dataDxfId="4"/>
     <tableColumn id="15" xr3:uid="{D96EE09E-B22B-4D75-AABE-AEBF7CE286A6}" name="Prix_Unitaire" dataDxfId="3"/>
     <tableColumn id="16" xr3:uid="{B1727D51-96B6-4015-83C5-EBCAD96E9834}" name="Prix Total" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{9A2C6D78-CE06-4E13-B8E1-0CB92B201156}" name="Semaine" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{9A2C6D78-CE06-4E13-B8E1-0CB92B201156}" name="Semaine" dataDxfId="1">
       <calculatedColumnFormula>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{83F3E9A5-7911-47C6-B543-07173CE7D4B5}" name="Mois" dataDxfId="1">
+    <tableColumn id="18" xr3:uid="{83F3E9A5-7911-47C6-B543-07173CE7D4B5}" name="Mois" dataDxfId="0">
       <calculatedColumnFormula>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1199,10 +1250,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:P89"/>
+  <dimension ref="A1:P102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="106" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="J82" zoomScale="106" zoomScaleNormal="103" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90:N102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5170,6 +5221,586 @@
         <v>septembre</v>
       </c>
     </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A90" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B90" t="s">
+        <v>31</v>
+      </c>
+      <c r="C90" t="s">
+        <v>32</v>
+      </c>
+      <c r="D90" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="F90" s="10">
+        <v>782406319</v>
+      </c>
+      <c r="G90" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H90" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I90" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J90" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K90" s="10"/>
+      <c r="L90" s="10"/>
+      <c r="M90" s="12"/>
+      <c r="N90" s="12"/>
+      <c r="O90" s="13" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+      <c r="P90" s="14" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>septembre</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A91" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B91" t="s">
+        <v>31</v>
+      </c>
+      <c r="C91" t="s">
+        <v>32</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="F91" s="10">
+        <v>782406319</v>
+      </c>
+      <c r="G91" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H91" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I91" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J91" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K91" s="10"/>
+      <c r="L91" s="10"/>
+      <c r="M91" s="12"/>
+      <c r="N91" s="12"/>
+      <c r="O91" s="13" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+      <c r="P91" s="14" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>septembre</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A92" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B92" t="s">
+        <v>31</v>
+      </c>
+      <c r="C92" t="s">
+        <v>32</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F92" s="10">
+        <v>770554097</v>
+      </c>
+      <c r="G92" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H92" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I92" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J92" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K92" s="10"/>
+      <c r="L92" s="10"/>
+      <c r="M92" s="12"/>
+      <c r="N92" s="12"/>
+      <c r="O92" s="13" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+      <c r="P92" s="14" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>septembre</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A93" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B93" t="s">
+        <v>31</v>
+      </c>
+      <c r="C93" t="s">
+        <v>32</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="F93" s="10">
+        <v>776135597</v>
+      </c>
+      <c r="G93" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H93" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I93" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J93" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K93" s="10"/>
+      <c r="L93" s="10"/>
+      <c r="M93" s="12"/>
+      <c r="N93" s="12"/>
+      <c r="O93" s="13" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+      <c r="P93" s="14" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>septembre</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A94" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B94" t="s">
+        <v>31</v>
+      </c>
+      <c r="C94" t="s">
+        <v>32</v>
+      </c>
+      <c r="D94" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="F94" s="10">
+        <v>775564374</v>
+      </c>
+      <c r="G94" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H94" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I94" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J94" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K94" s="10"/>
+      <c r="L94" s="10"/>
+      <c r="M94" s="12"/>
+      <c r="N94" s="12"/>
+      <c r="O94" s="13" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+      <c r="P94" s="14" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>septembre</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A95" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B95" t="s">
+        <v>31</v>
+      </c>
+      <c r="C95" t="s">
+        <v>32</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F95" s="10">
+        <v>775744949</v>
+      </c>
+      <c r="G95" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H95" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I95" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J95" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K95" s="10"/>
+      <c r="L95" s="10"/>
+      <c r="M95" s="12"/>
+      <c r="N95" s="12"/>
+      <c r="O95" s="13" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+      <c r="P95" s="14" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>septembre</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A96" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B96" t="s">
+        <v>31</v>
+      </c>
+      <c r="C96" t="s">
+        <v>32</v>
+      </c>
+      <c r="D96" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="F96" s="10">
+        <v>775711190</v>
+      </c>
+      <c r="G96" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H96" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I96" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J96" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K96" s="10"/>
+      <c r="L96" s="10"/>
+      <c r="M96" s="12"/>
+      <c r="N96" s="12"/>
+      <c r="O96" s="13" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+      <c r="P96" s="14" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>septembre</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A97" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B97" t="s">
+        <v>31</v>
+      </c>
+      <c r="C97" t="s">
+        <v>32</v>
+      </c>
+      <c r="D97" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F97" s="10">
+        <v>774118519</v>
+      </c>
+      <c r="G97" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H97" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I97" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J97" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K97" s="10"/>
+      <c r="L97" s="10"/>
+      <c r="M97" s="12"/>
+      <c r="N97" s="12"/>
+      <c r="O97" s="13" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+      <c r="P97" s="14" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>septembre</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A98" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B98" t="s">
+        <v>31</v>
+      </c>
+      <c r="C98" t="s">
+        <v>32</v>
+      </c>
+      <c r="D98" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="F98" s="10">
+        <v>779890912</v>
+      </c>
+      <c r="G98" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H98" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I98" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J98" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K98" s="10"/>
+      <c r="L98" s="10"/>
+      <c r="M98" s="12"/>
+      <c r="N98" s="12"/>
+      <c r="O98" s="13" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+      <c r="P98" s="14" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>septembre</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A99" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B99" t="s">
+        <v>31</v>
+      </c>
+      <c r="C99" t="s">
+        <v>32</v>
+      </c>
+      <c r="D99" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="F99" s="10">
+        <v>774216339</v>
+      </c>
+      <c r="G99" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H99" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I99" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J99" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="K99" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L99" s="10">
+        <v>25</v>
+      </c>
+      <c r="M99" s="12">
+        <v>9750</v>
+      </c>
+      <c r="N99" s="12">
+        <v>243750</v>
+      </c>
+      <c r="O99" s="13" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+      <c r="P99" s="14" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>septembre</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A100" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B100" t="s">
+        <v>31</v>
+      </c>
+      <c r="C100" t="s">
+        <v>32</v>
+      </c>
+      <c r="D100" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E100" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="F100" s="10">
+        <v>779890912</v>
+      </c>
+      <c r="G100" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H100" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I100" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J100" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K100" s="10"/>
+      <c r="L100" s="10"/>
+      <c r="M100" s="12"/>
+      <c r="N100" s="12"/>
+      <c r="O100" s="13" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+      <c r="P100" s="14" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>septembre</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A101" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B101" t="s">
+        <v>31</v>
+      </c>
+      <c r="C101" t="s">
+        <v>32</v>
+      </c>
+      <c r="D101" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="F101" s="10">
+        <v>779204232</v>
+      </c>
+      <c r="G101" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H101" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I101" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J101" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="K101" s="10"/>
+      <c r="L101" s="10"/>
+      <c r="M101" s="12"/>
+      <c r="N101" s="12"/>
+      <c r="O101" s="13" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+      <c r="P101" s="14" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>septembre</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A102" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B102" t="s">
+        <v>31</v>
+      </c>
+      <c r="C102" t="s">
+        <v>32</v>
+      </c>
+      <c r="D102" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E102" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="F102" s="10">
+        <v>775386609</v>
+      </c>
+      <c r="G102" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H102" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I102" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J102" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K102" s="10"/>
+      <c r="L102" s="10"/>
+      <c r="M102" s="12"/>
+      <c r="N102" s="12"/>
+      <c r="O102" s="13" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+      <c r="P102" s="14" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>septembre</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Rapport du 08 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_RZ.xlsx
+++ b/Donnees_RZ.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE17B4B-4CD5-4F3C-B517-7EB052769876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE04908D-3B6E-40F8-A9A7-FFFDDA98E99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="378">
   <si>
     <t>Date</t>
   </si>
@@ -1153,6 +1166,9 @@
   </si>
   <si>
     <t>Ya aussi du restant</t>
+  </si>
+  <si>
+    <t>Semaine</t>
   </si>
 </sst>
 </file>
@@ -1203,7 +1219,384 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1214,6 +1607,37 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE8635A2-CE0D-4957-87E4-9A74426F68AC}" name="Tableau1" displayName="Tableau1" ref="A1:T111" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2">
+  <autoFilter ref="A1:T111" xr:uid="{EE8635A2-CE0D-4957-87E4-9A74426F68AC}"/>
+  <tableColumns count="20">
+    <tableColumn id="1" xr3:uid="{989F4776-8306-4848-ADB0-7D708A60AE96}" name="Date" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{4FDB193D-9F39-4F40-84A0-1EC92B7891B7}" name="Prenom_Nom_RZ" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{140A8319-B7DC-456F-998D-7DA762539B3E}" name="zone" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{0A420A9B-0431-414E-9A86-B8D79565E26F}" name="secteur" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{2B40B431-D830-407F-94DB-A33AB15E83A5}" name="Nom_du_magasin" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{94E4AFE2-FE79-40AE-85E7-1B4534F71F85}" name="Telephone_Client" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{3BA6D4AA-DE73-4524-821F-1D73A7BB5333}" name="Type" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{A9450410-AA25-45B3-ABEC-8B8649FB49CD}" name="Point_de_Vente" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{8F45C5D1-4968-4D78-BA86-4177231C4069}" name="Operation" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{5CCD6703-6D47-4CE5-8580-5469D1F6CC1D}" name="Commentaire" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{11DEBA0F-DBE6-4331-A070-B5B0C3A499ED}" name="Latitude" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{8FBAAADD-88C0-469F-A5A1-AE6FFFC8B26B}" name="Longitude" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{1EB5390A-4758-4E0E-80A1-DF984D5590A0}" name="Altitude" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{7918C3D3-F54B-4F0E-AE73-2DED65121736}" name="Precision" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{9A255AAB-A336-4427-9D07-FD11211FB8EB}" name="start_geopoint" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{A5EC9131-A139-4028-A433-EFB201A6E9DA}" name="Telephone_RZ" dataDxfId="6"/>
+    <tableColumn id="17" xr3:uid="{8772C6F5-0612-4753-B48A-75DD29A41FBE}" name="Produit" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{3169A221-C213-405E-B3F0-7F17CA62807B}" name="Quantites" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{1446AB15-0F9D-4B64-B62B-927584229A9B}" name="Prix_Unitaire" dataDxfId="3"/>
+    <tableColumn id="20" xr3:uid="{A8F1F27D-F2A1-44A9-AD3C-0FEBB35E5EF3}" name="Semaine" dataDxfId="0">
+      <calculatedColumnFormula>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1533,9 +1957,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S111"/>
+  <dimension ref="A1:T111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1544,7 +1970,7 @@
     <col min="3" max="3" width="17.1328125" customWidth="1"/>
     <col min="4" max="4" width="18.59765625" customWidth="1"/>
     <col min="5" max="5" width="26.9296875" customWidth="1"/>
-    <col min="6" max="6" width="12.1328125" customWidth="1"/>
+    <col min="6" max="6" width="17.1328125" customWidth="1"/>
     <col min="7" max="7" width="13.19921875" customWidth="1"/>
     <col min="8" max="8" width="21.796875" customWidth="1"/>
     <col min="9" max="9" width="12.46484375" customWidth="1"/>
@@ -1552,15 +1978,15 @@
     <col min="11" max="11" width="12.73046875" customWidth="1"/>
     <col min="12" max="12" width="13.46484375" customWidth="1"/>
     <col min="13" max="13" width="21.33203125" customWidth="1"/>
-    <col min="14" max="14" width="7.86328125" customWidth="1"/>
+    <col min="14" max="14" width="10.1328125" customWidth="1"/>
     <col min="15" max="15" width="55.06640625" customWidth="1"/>
-    <col min="16" max="16" width="12.1328125" customWidth="1"/>
+    <col min="16" max="16" width="14.59765625" customWidth="1"/>
     <col min="17" max="17" width="33.86328125" customWidth="1"/>
-    <col min="18" max="18" width="4.796875" customWidth="1"/>
-    <col min="19" max="19" width="7.19921875" customWidth="1"/>
+    <col min="18" max="18" width="10.59765625" customWidth="1"/>
+    <col min="19" max="19" width="13.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1618,8 +2044,11 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T1" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>45908</v>
       </c>
@@ -1671,8 +2100,12 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T2" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>45908</v>
       </c>
@@ -1714,8 +2147,12 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T3" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>45908</v>
       </c>
@@ -1757,8 +2194,12 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T4" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>45908</v>
       </c>
@@ -1810,8 +2251,12 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T5" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>45908</v>
       </c>
@@ -1863,8 +2308,12 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T6" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>45908</v>
       </c>
@@ -1916,8 +2365,12 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T7" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>45908</v>
       </c>
@@ -1969,8 +2422,12 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T8" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>45908</v>
       </c>
@@ -2022,8 +2479,12 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T9" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>45908</v>
       </c>
@@ -2065,8 +2526,12 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T10" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>45908</v>
       </c>
@@ -2118,8 +2583,12 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T11" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>45908</v>
       </c>
@@ -2161,8 +2630,12 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T12" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>45908</v>
       </c>
@@ -2214,8 +2687,12 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T13" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>45908</v>
       </c>
@@ -2257,8 +2734,12 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T14" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>45908</v>
       </c>
@@ -2310,8 +2791,12 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T15" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>45908</v>
       </c>
@@ -2363,8 +2848,12 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T16" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>45908</v>
       </c>
@@ -2412,8 +2901,12 @@
       <c r="S17" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T17" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <v>45908</v>
       </c>
@@ -2461,8 +2954,12 @@
       <c r="S18" s="1">
         <v>19500</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T18" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>45908</v>
       </c>
@@ -2510,8 +3007,12 @@
       <c r="S19" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T19" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>45908</v>
       </c>
@@ -2563,8 +3064,12 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T20" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>45908</v>
       </c>
@@ -2622,8 +3127,12 @@
       <c r="S21" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T21" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>45908</v>
       </c>
@@ -2675,8 +3184,12 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T22" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>45908</v>
       </c>
@@ -2728,8 +3241,12 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T23" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>45908</v>
       </c>
@@ -2781,8 +3298,12 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T24" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>45908</v>
       </c>
@@ -2834,8 +3355,12 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T25" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>45908</v>
       </c>
@@ -2893,8 +3418,12 @@
       <c r="S26" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T26" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>45908</v>
       </c>
@@ -2946,8 +3475,12 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T27" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>45907</v>
       </c>
@@ -2995,8 +3528,12 @@
       <c r="S28" s="1">
         <v>33500</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T28" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>45907</v>
       </c>
@@ -3044,8 +3581,12 @@
       <c r="S29" s="1">
         <v>33500</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T29" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>45908</v>
       </c>
@@ -3093,8 +3634,12 @@
       <c r="S30" s="1">
         <v>19500</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T30" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>45908</v>
       </c>
@@ -3142,8 +3687,12 @@
       <c r="S31" s="1">
         <v>19500</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T31" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <v>45908</v>
       </c>
@@ -3191,8 +3740,12 @@
       <c r="S32" s="1">
         <v>19500</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T32" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
         <v>45908</v>
       </c>
@@ -3240,8 +3793,12 @@
       <c r="S33" s="1">
         <v>19500</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T33" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A34" s="2">
         <v>45908</v>
       </c>
@@ -3283,8 +3840,12 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T34" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
         <v>45908</v>
       </c>
@@ -3326,8 +3887,12 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T35" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A36" s="2">
         <v>45908</v>
       </c>
@@ -3379,8 +3944,12 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T36" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
         <v>45908</v>
       </c>
@@ -3438,8 +4007,12 @@
       <c r="S37" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T37" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A38" s="2">
         <v>45908</v>
       </c>
@@ -3497,8 +4070,12 @@
       <c r="S38" s="1">
         <v>31000</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T38" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A39" s="2">
         <v>45908</v>
       </c>
@@ -3556,8 +4133,12 @@
       <c r="S39" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T39" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A40" s="2">
         <v>45908</v>
       </c>
@@ -3615,8 +4196,12 @@
       <c r="S40" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T40" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A41" s="2">
         <v>45908</v>
       </c>
@@ -3674,8 +4259,12 @@
       <c r="S41" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T41" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
         <v>45908</v>
       </c>
@@ -3727,8 +4316,12 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T42" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <v>45908</v>
       </c>
@@ -3780,8 +4373,12 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T43" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
         <v>45908</v>
       </c>
@@ -3833,8 +4430,12 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T44" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
         <v>45908</v>
       </c>
@@ -3892,8 +4493,12 @@
       <c r="S45" s="1">
         <v>12250</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T45" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A46" s="2">
         <v>45908</v>
       </c>
@@ -3951,8 +4556,12 @@
       <c r="S46" s="1">
         <v>12250</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T46" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A47" s="2">
         <v>45908</v>
       </c>
@@ -4004,8 +4613,12 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T47" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
         <v>45908</v>
       </c>
@@ -4057,8 +4670,12 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T48" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
         <v>45908</v>
       </c>
@@ -4110,8 +4727,12 @@
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T49" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
         <v>45908</v>
       </c>
@@ -4163,8 +4784,12 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T50" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
         <v>45908</v>
       </c>
@@ -4216,8 +4841,12 @@
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T51" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
         <v>45908</v>
       </c>
@@ -4269,8 +4898,12 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T52" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
         <v>45908</v>
       </c>
@@ -4312,8 +4945,12 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T53" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
         <v>45908</v>
       </c>
@@ -4355,8 +4992,12 @@
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T54" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
         <v>45908</v>
       </c>
@@ -4398,8 +5039,12 @@
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T55" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
         <v>45908</v>
       </c>
@@ -4441,8 +5086,12 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T56" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
         <v>45908</v>
       </c>
@@ -4484,8 +5133,12 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T57" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
         <v>45908</v>
       </c>
@@ -4527,8 +5180,12 @@
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T58" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A59" s="2">
         <v>45908</v>
       </c>
@@ -4576,8 +5233,12 @@
       <c r="S59" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T59" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A60" s="2">
         <v>45908</v>
       </c>
@@ -4619,8 +5280,12 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T60" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A61" s="2">
         <v>45908</v>
       </c>
@@ -4662,8 +5327,12 @@
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
       <c r="S61" s="1"/>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T61" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A62" s="2">
         <v>45908</v>
       </c>
@@ -4711,8 +5380,12 @@
       <c r="S62" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T62" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A63" s="2">
         <v>45908</v>
       </c>
@@ -4754,8 +5427,12 @@
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
       <c r="S63" s="1"/>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T63" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A64" s="2">
         <v>45908</v>
       </c>
@@ -4797,8 +5474,12 @@
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
       <c r="S64" s="1"/>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T64" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A65" s="2">
         <v>45908</v>
       </c>
@@ -4840,8 +5521,12 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
       <c r="S65" s="1"/>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T65" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A66" s="2">
         <v>45908</v>
       </c>
@@ -4883,8 +5568,12 @@
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
       <c r="S66" s="1"/>
-    </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T66" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A67" s="2">
         <v>45908</v>
       </c>
@@ -4926,8 +5615,12 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
       <c r="S67" s="1"/>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T67" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A68" s="2">
         <v>45908</v>
       </c>
@@ -4969,8 +5662,12 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
       <c r="S68" s="1"/>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T68" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A69" s="2">
         <v>45908</v>
       </c>
@@ -5012,8 +5709,12 @@
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
       <c r="S69" s="1"/>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T69" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A70" s="2">
         <v>45908</v>
       </c>
@@ -5061,8 +5762,12 @@
       <c r="S70" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T70" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A71" s="2">
         <v>45908</v>
       </c>
@@ -5104,8 +5809,12 @@
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
       <c r="S71" s="1"/>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T71" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A72" s="2">
         <v>45908</v>
       </c>
@@ -5147,8 +5856,12 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
       <c r="S72" s="1"/>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T72" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A73" s="2">
         <v>45908</v>
       </c>
@@ -5190,8 +5903,12 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
       <c r="S73" s="1"/>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T73" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A74" s="2">
         <v>45908</v>
       </c>
@@ -5233,8 +5950,12 @@
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
       <c r="S74" s="1"/>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T74" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A75" s="2">
         <v>45908</v>
       </c>
@@ -5276,8 +5997,12 @@
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
       <c r="S75" s="1"/>
-    </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T75" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A76" s="2">
         <v>45908</v>
       </c>
@@ -5319,8 +6044,12 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
       <c r="S76" s="1"/>
-    </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T76" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A77" s="2">
         <v>45908</v>
       </c>
@@ -5362,8 +6091,12 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
       <c r="S77" s="1"/>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T77" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A78" s="2">
         <v>45908</v>
       </c>
@@ -5411,8 +6144,12 @@
       <c r="S78" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T78" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A79" s="2">
         <v>45908</v>
       </c>
@@ -5460,8 +6197,12 @@
       <c r="S79" s="1">
         <v>9750</v>
       </c>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T79" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A80" s="2">
         <v>45908</v>
       </c>
@@ -5503,8 +6244,12 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
       <c r="S80" s="1"/>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T80" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A81" s="2">
         <v>45908</v>
       </c>
@@ -5546,8 +6291,12 @@
       <c r="Q81" s="1"/>
       <c r="R81" s="1"/>
       <c r="S81" s="1"/>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T81" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A82" s="2">
         <v>45908</v>
       </c>
@@ -5595,8 +6344,12 @@
       <c r="S82" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T82" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A83" s="2">
         <v>45908</v>
       </c>
@@ -5644,8 +6397,12 @@
       <c r="S83" s="1">
         <v>9750</v>
       </c>
-    </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T83" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A84" s="2">
         <v>45908</v>
       </c>
@@ -5687,8 +6444,12 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
       <c r="S84" s="1"/>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T84" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A85" s="2">
         <v>45908</v>
       </c>
@@ -5730,8 +6491,12 @@
       <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
       <c r="S85" s="1"/>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T85" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A86" s="2">
         <v>45908</v>
       </c>
@@ -5773,8 +6538,12 @@
       <c r="Q86" s="1"/>
       <c r="R86" s="1"/>
       <c r="S86" s="1"/>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T86" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A87" s="2">
         <v>45908</v>
       </c>
@@ -5816,8 +6585,12 @@
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
       <c r="S87" s="1"/>
-    </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T87" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A88" s="2">
         <v>45908</v>
       </c>
@@ -5865,8 +6638,12 @@
       <c r="S88" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T88" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A89" s="2">
         <v>45908</v>
       </c>
@@ -5914,8 +6691,12 @@
       <c r="S89" s="1">
         <v>9750</v>
       </c>
-    </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T89" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A90" s="2">
         <v>45908</v>
       </c>
@@ -5963,8 +6744,12 @@
       <c r="S90" s="1">
         <v>19500</v>
       </c>
-    </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T90" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A91" s="2">
         <v>45908</v>
       </c>
@@ -6012,8 +6797,12 @@
       <c r="S91" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T91" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A92" s="2">
         <v>45908</v>
       </c>
@@ -6061,8 +6850,12 @@
       <c r="S92" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T92" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A93" s="2">
         <v>45908</v>
       </c>
@@ -6104,8 +6897,12 @@
       <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
       <c r="S93" s="1"/>
-    </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T93" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A94" s="2">
         <v>45908</v>
       </c>
@@ -6147,8 +6944,12 @@
       <c r="Q94" s="1"/>
       <c r="R94" s="1"/>
       <c r="S94" s="1"/>
-    </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T94" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A95" s="2">
         <v>45908</v>
       </c>
@@ -6190,8 +6991,12 @@
       <c r="Q95" s="1"/>
       <c r="R95" s="1"/>
       <c r="S95" s="1"/>
-    </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T95" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A96" s="2">
         <v>45908</v>
       </c>
@@ -6233,8 +7038,12 @@
       <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
       <c r="S96" s="1"/>
-    </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T96" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A97" s="2">
         <v>45908</v>
       </c>
@@ -6276,8 +7085,12 @@
       <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
       <c r="S97" s="1"/>
-    </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T97" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A98" s="2">
         <v>45908</v>
       </c>
@@ -6319,8 +7132,12 @@
       <c r="Q98" s="1"/>
       <c r="R98" s="1"/>
       <c r="S98" s="1"/>
-    </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T98" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A99" s="2">
         <v>45908</v>
       </c>
@@ -6362,8 +7179,12 @@
       <c r="Q99" s="1"/>
       <c r="R99" s="1"/>
       <c r="S99" s="1"/>
-    </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T99" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A100" s="2">
         <v>45908</v>
       </c>
@@ -6405,8 +7226,12 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
       <c r="S100" s="1"/>
-    </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T100" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A101" s="2">
         <v>45908</v>
       </c>
@@ -6454,8 +7279,12 @@
       <c r="S101" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T101" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A102" s="2">
         <v>45908</v>
       </c>
@@ -6497,8 +7326,12 @@
       <c r="Q102" s="1"/>
       <c r="R102" s="1"/>
       <c r="S102" s="1"/>
-    </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T102" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A103" s="2">
         <v>45908</v>
       </c>
@@ -6540,8 +7373,12 @@
       <c r="Q103" s="1"/>
       <c r="R103" s="1"/>
       <c r="S103" s="1"/>
-    </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T103" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A104" s="2">
         <v>45908</v>
       </c>
@@ -6583,8 +7420,12 @@
       <c r="Q104" s="1"/>
       <c r="R104" s="1"/>
       <c r="S104" s="1"/>
-    </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T104" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A105" s="2">
         <v>45908</v>
       </c>
@@ -6632,8 +7473,12 @@
       <c r="S105" s="1">
         <v>26000</v>
       </c>
-    </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T105" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A106" s="2">
         <v>45908</v>
       </c>
@@ -6675,8 +7520,12 @@
       <c r="Q106" s="1"/>
       <c r="R106" s="1"/>
       <c r="S106" s="1"/>
-    </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T106" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A107" s="2">
         <v>45908</v>
       </c>
@@ -6724,8 +7573,12 @@
       <c r="S107" s="1">
         <v>7500</v>
       </c>
-    </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T107" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A108" s="2">
         <v>45908</v>
       </c>
@@ -6773,8 +7626,12 @@
       <c r="S108" s="1">
         <v>7500</v>
       </c>
-    </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T108" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A109" s="2">
         <v>45907</v>
       </c>
@@ -6832,8 +7689,12 @@
       <c r="S109" s="1">
         <v>7500</v>
       </c>
-    </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T109" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S36</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A110" s="2">
         <v>45908</v>
       </c>
@@ -6875,8 +7736,12 @@
       <c r="Q110" s="1"/>
       <c r="R110" s="1"/>
       <c r="S110" s="1"/>
-    </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="T110" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A111" s="2">
         <v>45908</v>
       </c>
@@ -6918,8 +7783,15 @@
       <c r="Q111" s="1"/>
       <c r="R111" s="1"/>
       <c r="S111" s="1"/>
+      <c r="T111" s="1" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Tableau1[[#This Row],[Date]])</f>
+        <v>S37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rapport du 13 Septembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_RZ.xlsx
+++ b/Donnees_RZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBD2690-76C4-46E8-85C1-7E3E2E89D768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F817983-2BA3-465F-8974-48347E996234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2672,8 +2672,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:P389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="106" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="B394" sqref="B394"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="106" zoomScaleNormal="103" workbookViewId="0">
+      <selection activeCell="M78" sqref="M78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4088,11 +4088,11 @@
         <v>2</v>
       </c>
       <c r="M29" s="10">
+        <v>9750</v>
+      </c>
+      <c r="N29" s="12">
+        <f>Semaine_1[[#This Row],[Prix_Unitaire]]*Semaine_1[[#This Row],[Quantites]]</f>
         <v>19500</v>
-      </c>
-      <c r="N29" s="12">
-        <f>Semaine_1[[#This Row],[Prix_Unitaire]]*Semaine_1[[#This Row],[Quantites]]</f>
-        <v>39000</v>
       </c>
       <c r="O29" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>

</xml_diff>

<commit_message>
Rapport des RZ du 06 Octobre 2025
</commit_message>
<xml_diff>
--- a/Donnees_RZ.xlsx
+++ b/Donnees_RZ.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ADE437-91BE-45D9-AFC8-8B2D05209E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA7202D-A597-4AB9-96EF-C845A78CE0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -234,6 +234,42 @@
   </si>
   <si>
     <t>Modou boye</t>
+  </si>
+  <si>
+    <t>Seynabou SOW</t>
+  </si>
+  <si>
+    <t>CASTOR</t>
+  </si>
+  <si>
+    <t>Castor</t>
+  </si>
+  <si>
+    <t>Ndioguou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merci beaucoup </t>
+  </si>
+  <si>
+    <t>MATAR LY</t>
+  </si>
+  <si>
+    <t>Marché Bou Bess</t>
+  </si>
+  <si>
+    <t>MOUSTAPHA DIALLO</t>
+  </si>
+  <si>
+    <t>Café pot Refraish 50g</t>
+  </si>
+  <si>
+    <t>MOUSTAPHA MBAO</t>
+  </si>
+  <si>
+    <t>Alpha ba</t>
+  </si>
+  <si>
+    <t>Merci beaucoup</t>
   </si>
 </sst>
 </file>
@@ -630,8 +666,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P19" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A1:P19" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P26" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A1:P26" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -947,10 +983,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:N19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1647,313 +1683,677 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A14" s="13">
+      <c r="A14" s="9">
         <v>45933</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="10">
         <v>775602981</v>
       </c>
-      <c r="G14" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="15" t="s">
+      <c r="G14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="K14" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L14" s="10">
         <v>25</v>
       </c>
-      <c r="M14" s="16">
+      <c r="M14" s="12">
         <v>6000</v>
       </c>
-      <c r="N14" s="16">
+      <c r="N14" s="12">
         <v>150000</v>
       </c>
-      <c r="O14" s="17" t="str">
+      <c r="O14" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S40</v>
       </c>
-      <c r="P14" s="18" t="str">
+      <c r="P14" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A15" s="13">
+      <c r="A15" s="9">
         <v>45933</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="10">
         <v>778195274</v>
       </c>
-      <c r="G15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="15" t="s">
+      <c r="G15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="K15" s="14" t="s">
+      <c r="K15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="10">
         <v>50</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15" s="12">
         <v>26000</v>
       </c>
-      <c r="N15" s="16">
+      <c r="N15" s="12">
         <v>1300000</v>
       </c>
-      <c r="O15" s="17" t="str">
+      <c r="O15" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S40</v>
       </c>
-      <c r="P15" s="18" t="str">
+      <c r="P15" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A16" s="13">
+      <c r="A16" s="9">
         <v>45933</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="10">
         <v>762974040</v>
       </c>
-      <c r="G16" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J16" s="15" t="s">
+      <c r="G16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K16" s="14" t="s">
+      <c r="K16" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="10">
         <v>25</v>
       </c>
-      <c r="M16" s="16">
+      <c r="M16" s="12">
         <v>26000</v>
       </c>
-      <c r="N16" s="16">
+      <c r="N16" s="12">
         <v>650000</v>
       </c>
-      <c r="O16" s="17" t="str">
+      <c r="O16" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S40</v>
       </c>
-      <c r="P16" s="18" t="str">
+      <c r="P16" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A17" s="13">
+      <c r="A17" s="9">
         <v>45933</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="10">
         <v>778056161</v>
       </c>
-      <c r="G17" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J17" s="15" t="s">
+      <c r="G17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="14">
+      <c r="L17" s="10">
         <v>25</v>
       </c>
-      <c r="M17" s="16">
+      <c r="M17" s="12">
         <v>26000</v>
       </c>
-      <c r="N17" s="16">
+      <c r="N17" s="12">
         <v>650000</v>
       </c>
-      <c r="O17" s="17" t="str">
+      <c r="O17" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S40</v>
       </c>
-      <c r="P17" s="18" t="str">
+      <c r="P17" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A18" s="13">
+      <c r="A18" s="9">
         <v>45933</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="10">
         <v>774216339</v>
       </c>
-      <c r="G18" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="15" t="s">
+      <c r="G18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K18" s="14" t="s">
+      <c r="K18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="14">
+      <c r="L18" s="10">
         <v>50</v>
       </c>
-      <c r="M18" s="16">
+      <c r="M18" s="12">
         <v>26000</v>
       </c>
-      <c r="N18" s="16">
+      <c r="N18" s="12">
         <v>1300000</v>
       </c>
-      <c r="O18" s="17" t="str">
+      <c r="O18" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S40</v>
       </c>
-      <c r="P18" s="18" t="str">
+      <c r="P18" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A19" s="13">
+      <c r="A19" s="9">
         <v>45933</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="10">
         <v>767379110</v>
       </c>
-      <c r="G19" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" s="15" t="s">
+      <c r="G19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K19" s="14" t="s">
+      <c r="K19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="10">
         <v>50</v>
       </c>
-      <c r="M19" s="16">
+      <c r="M19" s="12">
         <v>26000</v>
       </c>
-      <c r="N19" s="16">
+      <c r="N19" s="12">
         <v>1300000</v>
       </c>
-      <c r="O19" s="17" t="str">
+      <c r="O19" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S40</v>
       </c>
-      <c r="P19" s="18" t="str">
+      <c r="P19" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A20" s="13">
+        <v>45936</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="14">
+        <v>776634479</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="14">
+        <v>3</v>
+      </c>
+      <c r="M20" s="16">
+        <v>19500</v>
+      </c>
+      <c r="N20" s="16">
+        <v>58500</v>
+      </c>
+      <c r="O20" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P20" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A21" s="13">
+        <v>45936</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="14">
+        <v>773531341</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="14">
+        <v>200</v>
+      </c>
+      <c r="M21" s="16">
+        <v>26000</v>
+      </c>
+      <c r="N21" s="16">
+        <v>5200000</v>
+      </c>
+      <c r="O21" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P21" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A22" s="13">
+        <v>45936</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="14">
+        <v>784537895</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="14">
+        <v>25</v>
+      </c>
+      <c r="M22" s="16">
+        <v>19500</v>
+      </c>
+      <c r="N22" s="16">
+        <v>487500</v>
+      </c>
+      <c r="O22" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P22" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A23" s="13">
+        <v>45936</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="14">
+        <v>784537895</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="L23" s="14">
+        <v>25</v>
+      </c>
+      <c r="M23" s="16">
+        <v>9750</v>
+      </c>
+      <c r="N23" s="16">
+        <v>243750</v>
+      </c>
+      <c r="O23" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P23" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A24" s="13">
+        <v>45936</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="14">
+        <v>784537895</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" s="14">
+        <v>50</v>
+      </c>
+      <c r="M24" s="16">
+        <v>26000</v>
+      </c>
+      <c r="N24" s="16">
+        <v>1300000</v>
+      </c>
+      <c r="O24" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P24" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A25" s="13">
+        <v>45936</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="14">
+        <v>776503464</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="14">
+        <v>25</v>
+      </c>
+      <c r="M25" s="16">
+        <v>26000</v>
+      </c>
+      <c r="N25" s="16">
+        <v>650000</v>
+      </c>
+      <c r="O25" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P25" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A26" s="13">
+        <v>45936</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="14">
+        <v>773564759</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="L26" s="14">
+        <v>5</v>
+      </c>
+      <c r="M26" s="16">
+        <v>10250</v>
+      </c>
+      <c r="N26" s="16">
+        <v>51250</v>
+      </c>
+      <c r="O26" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P26" s="18" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>

</xml_diff>

<commit_message>
Modification Rapport de NGOUYE NDIAYE
</commit_message>
<xml_diff>
--- a/Donnees_RZ.xlsx
+++ b/Donnees_RZ.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA7202D-A597-4AB9-96EF-C845A78CE0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391E210D-921C-4B57-87C5-A010124F5232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semaine 1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -270,6 +270,18 @@
   </si>
   <si>
     <t>Merci beaucoup</t>
+  </si>
+  <si>
+    <t>Ngouye NDIAYE</t>
+  </si>
+  <si>
+    <t>PIKINE</t>
+  </si>
+  <si>
+    <t>Keur Mbaye Fall</t>
+  </si>
+  <si>
+    <t>Alassane Diallo</t>
   </si>
 </sst>
 </file>
@@ -666,8 +678,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P26" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A1:P26" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P27" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A1:P27" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P2">
     <sortCondition ref="A1:A2"/>
   </sortState>
@@ -983,10 +995,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:N26"/>
+    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1995,365 +2007,417 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A20" s="13">
+      <c r="A20" s="9">
         <v>45936</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="10">
         <v>776634479</v>
       </c>
-      <c r="G20" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" s="15" t="s">
+      <c r="G20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L20" s="14">
+      <c r="L20" s="10">
         <v>3</v>
       </c>
-      <c r="M20" s="16">
+      <c r="M20" s="12">
         <v>19500</v>
       </c>
-      <c r="N20" s="16">
+      <c r="N20" s="12">
         <v>58500</v>
       </c>
-      <c r="O20" s="17" t="str">
+      <c r="O20" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S41</v>
       </c>
-      <c r="P20" s="18" t="str">
+      <c r="P20" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A21" s="13">
+      <c r="A21" s="9">
         <v>45936</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="10">
         <v>773531341</v>
       </c>
-      <c r="G21" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J21" s="15" t="s">
+      <c r="G21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K21" s="14" t="s">
+      <c r="K21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="14">
+      <c r="L21" s="10">
         <v>200</v>
       </c>
-      <c r="M21" s="16">
+      <c r="M21" s="12">
         <v>26000</v>
       </c>
-      <c r="N21" s="16">
+      <c r="N21" s="12">
         <v>5200000</v>
       </c>
-      <c r="O21" s="17" t="str">
+      <c r="O21" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S41</v>
       </c>
-      <c r="P21" s="18" t="str">
+      <c r="P21" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A22" s="13">
+      <c r="A22" s="9">
         <v>45936</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="10">
         <v>784537895</v>
       </c>
-      <c r="G22" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J22" s="15" t="s">
+      <c r="G22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="14" t="s">
+      <c r="K22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="14">
+      <c r="L22" s="10">
         <v>25</v>
       </c>
-      <c r="M22" s="16">
+      <c r="M22" s="12">
         <v>19500</v>
       </c>
-      <c r="N22" s="16">
+      <c r="N22" s="12">
         <v>487500</v>
       </c>
-      <c r="O22" s="17" t="str">
+      <c r="O22" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S41</v>
       </c>
-      <c r="P22" s="18" t="str">
+      <c r="P22" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A23" s="13">
+      <c r="A23" s="9">
         <v>45936</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="10">
         <v>784537895</v>
       </c>
-      <c r="G23" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="15" t="s">
+      <c r="G23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K23" s="14" t="s">
+      <c r="K23" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="L23" s="14">
+      <c r="L23" s="10">
         <v>25</v>
       </c>
-      <c r="M23" s="16">
+      <c r="M23" s="12">
         <v>9750</v>
       </c>
-      <c r="N23" s="16">
+      <c r="N23" s="12">
         <v>243750</v>
       </c>
-      <c r="O23" s="17" t="str">
+      <c r="O23" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S41</v>
       </c>
-      <c r="P23" s="18" t="str">
+      <c r="P23" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A24" s="13">
+      <c r="A24" s="9">
         <v>45936</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="10">
         <v>784537895</v>
       </c>
-      <c r="G24" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24" s="15" t="s">
+      <c r="G24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K24" s="14" t="s">
+      <c r="K24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="14">
+      <c r="L24" s="10">
         <v>50</v>
       </c>
-      <c r="M24" s="16">
+      <c r="M24" s="12">
         <v>26000</v>
       </c>
-      <c r="N24" s="16">
+      <c r="N24" s="12">
         <v>1300000</v>
       </c>
-      <c r="O24" s="17" t="str">
+      <c r="O24" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S41</v>
       </c>
-      <c r="P24" s="18" t="str">
+      <c r="P24" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A25" s="13">
+      <c r="A25" s="9">
         <v>45936</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="10">
         <v>776503464</v>
       </c>
-      <c r="G25" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J25" s="15" t="s">
+      <c r="G25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K25" s="14" t="s">
+      <c r="K25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L25" s="14">
+      <c r="L25" s="10">
         <v>25</v>
       </c>
-      <c r="M25" s="16">
+      <c r="M25" s="12">
         <v>26000</v>
       </c>
-      <c r="N25" s="16">
+      <c r="N25" s="12">
         <v>650000</v>
       </c>
-      <c r="O25" s="17" t="str">
+      <c r="O25" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S41</v>
       </c>
-      <c r="P25" s="18" t="str">
+      <c r="P25" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A26" s="13">
+      <c r="A26" s="9">
         <v>45936</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="10">
         <v>773564759</v>
       </c>
-      <c r="G26" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J26" s="15" t="s">
+      <c r="G26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="K26" s="14" t="s">
+      <c r="K26" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="L26" s="14">
-        <v>5</v>
-      </c>
-      <c r="M26" s="16">
+      <c r="L26" s="10">
+        <v>3</v>
+      </c>
+      <c r="M26" s="12">
         <v>10250</v>
       </c>
-      <c r="N26" s="16">
-        <v>51250</v>
-      </c>
-      <c r="O26" s="17" t="str">
+      <c r="N26" s="12">
+        <v>30750</v>
+      </c>
+      <c r="O26" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S41</v>
       </c>
-      <c r="P26" s="18" t="str">
+      <c r="P26" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A27" s="13">
+        <v>45936</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="14">
+        <v>772289185</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L27" s="14">
+        <v>25</v>
+      </c>
+      <c r="M27" s="16">
+        <v>26000</v>
+      </c>
+      <c r="N27" s="16">
+        <v>650000</v>
+      </c>
+      <c r="O27" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P27" s="18" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>

</xml_diff>

<commit_message>
Modification du prix de Altimo 1,5g
</commit_message>
<xml_diff>
--- a/Donnees_RZ.xlsx
+++ b/Donnees_RZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE13E78A-85DD-45DE-AE49-282EDA0E5374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD31F62F-BC99-42BF-A006-AE6D58E7BBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -602,16 +602,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1222,8 +1212,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:P97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="M99" sqref="M99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4364,1925 +4354,1925 @@
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A61" s="13">
+      <c r="A61" s="9">
         <v>45940</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="C61" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="D61" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="E61" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F61" s="14">
+      <c r="F61" s="10">
         <v>768059355</v>
       </c>
-      <c r="G61" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H61" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I61" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J61" s="15" t="s">
+      <c r="G61" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H61" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I61" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J61" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K61" s="14" t="s">
+      <c r="K61" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="L61" s="14">
+      <c r="L61" s="10">
         <v>50</v>
       </c>
-      <c r="M61" s="16">
+      <c r="M61" s="12">
         <v>9750</v>
       </c>
-      <c r="N61" s="16">
+      <c r="N61" s="12">
         <v>487500</v>
       </c>
-      <c r="O61" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P61" s="18" t="str">
+      <c r="O61" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P61" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A62" s="13">
+      <c r="A62" s="9">
         <v>45940</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="C62" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D62" s="14" t="s">
+      <c r="D62" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E62" s="14" t="s">
+      <c r="E62" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="F62" s="14">
+      <c r="F62" s="10">
         <v>777132186</v>
       </c>
-      <c r="G62" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H62" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I62" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J62" s="15" t="s">
+      <c r="G62" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I62" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J62" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K62" s="14" t="s">
+      <c r="K62" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="L62" s="14">
+      <c r="L62" s="10">
         <v>1</v>
       </c>
-      <c r="M62" s="16">
+      <c r="M62" s="12">
         <v>12500</v>
       </c>
-      <c r="N62" s="16">
+      <c r="N62" s="12">
         <v>12500</v>
       </c>
-      <c r="O62" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P62" s="18" t="str">
+      <c r="O62" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P62" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A63" s="13">
+      <c r="A63" s="9">
         <v>45940</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="14" t="s">
+      <c r="C63" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D63" s="14" t="s">
+      <c r="D63" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E63" s="14" t="s">
+      <c r="E63" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="F63" s="14">
+      <c r="F63" s="10">
         <v>777132186</v>
       </c>
-      <c r="G63" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H63" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I63" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J63" s="15" t="s">
+      <c r="G63" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I63" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J63" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K63" s="14" t="s">
+      <c r="K63" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="L63" s="14">
+      <c r="L63" s="10">
         <v>1</v>
       </c>
-      <c r="M63" s="16">
+      <c r="M63" s="12">
         <v>12500</v>
       </c>
-      <c r="N63" s="16">
+      <c r="N63" s="12">
         <v>12500</v>
       </c>
-      <c r="O63" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P63" s="18" t="str">
+      <c r="O63" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P63" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A64" s="13">
+      <c r="A64" s="9">
         <v>45940</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="C64" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D64" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E64" s="14" t="s">
+      <c r="E64" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="F64" s="14">
+      <c r="F64" s="10">
         <v>777132186</v>
       </c>
-      <c r="G64" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H64" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I64" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J64" s="15" t="s">
+      <c r="G64" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H64" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J64" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K64" s="14" t="s">
+      <c r="K64" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="L64" s="14">
+      <c r="L64" s="10">
         <v>1</v>
       </c>
-      <c r="M64" s="16">
+      <c r="M64" s="12">
         <v>15500</v>
       </c>
-      <c r="N64" s="16">
+      <c r="N64" s="12">
         <v>15500</v>
       </c>
-      <c r="O64" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P64" s="18" t="str">
+      <c r="O64" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P64" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A65" s="13">
+      <c r="A65" s="9">
         <v>45940</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C65" s="14" t="s">
+      <c r="C65" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D65" s="14" t="s">
+      <c r="D65" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E65" s="14" t="s">
+      <c r="E65" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="F65" s="14">
+      <c r="F65" s="10">
         <v>777132186</v>
       </c>
-      <c r="G65" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H65" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I65" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J65" s="15" t="s">
+      <c r="G65" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H65" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J65" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K65" s="14" t="s">
+      <c r="K65" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="L65" s="14">
+      <c r="L65" s="10">
         <v>1</v>
       </c>
-      <c r="M65" s="16">
+      <c r="M65" s="12">
         <v>15500</v>
       </c>
-      <c r="N65" s="16">
+      <c r="N65" s="12">
         <v>15500</v>
       </c>
-      <c r="O65" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P65" s="18" t="str">
+      <c r="O65" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P65" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A66" s="13">
+      <c r="A66" s="9">
         <v>45940</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C66" s="14" t="s">
+      <c r="C66" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D66" s="14" t="s">
+      <c r="D66" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E66" s="14" t="s">
+      <c r="E66" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="F66" s="14">
+      <c r="F66" s="10">
         <v>781532059</v>
       </c>
-      <c r="G66" s="14" t="s">
+      <c r="G66" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="H66" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I66" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J66" s="15" t="s">
+      <c r="H66" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J66" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K66" s="14" t="s">
+      <c r="K66" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="L66" s="14">
+      <c r="L66" s="10">
         <v>1</v>
       </c>
-      <c r="M66" s="16">
+      <c r="M66" s="12">
         <v>15000</v>
       </c>
-      <c r="N66" s="16">
+      <c r="N66" s="12">
         <v>15000</v>
       </c>
-      <c r="O66" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P66" s="18" t="str">
+      <c r="O66" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P66" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A67" s="13">
+      <c r="A67" s="9">
         <v>45940</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C67" s="14" t="s">
+      <c r="C67" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D67" s="14" t="s">
+      <c r="D67" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E67" s="14" t="s">
+      <c r="E67" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="F67" s="14">
+      <c r="F67" s="10">
         <v>781532059</v>
       </c>
-      <c r="G67" s="14" t="s">
+      <c r="G67" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="H67" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I67" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J67" s="15" t="s">
+      <c r="H67" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J67" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K67" s="14" t="s">
+      <c r="K67" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="L67" s="14">
+      <c r="L67" s="10">
         <v>1</v>
       </c>
-      <c r="M67" s="16">
+      <c r="M67" s="12">
         <v>15500</v>
       </c>
-      <c r="N67" s="16">
+      <c r="N67" s="12">
         <v>15500</v>
       </c>
-      <c r="O67" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P67" s="18" t="str">
+      <c r="O67" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P67" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A68" s="13">
+      <c r="A68" s="9">
         <v>45940</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B68" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C68" s="14" t="s">
+      <c r="C68" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D68" s="14" t="s">
+      <c r="D68" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E68" s="14" t="s">
+      <c r="E68" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F68" s="14">
+      <c r="F68" s="10">
         <v>778704739</v>
       </c>
-      <c r="G68" s="14" t="s">
+      <c r="G68" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="H68" s="14" t="s">
+      <c r="H68" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="I68" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J68" s="15" t="s">
+      <c r="I68" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J68" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K68" s="14" t="s">
+      <c r="K68" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="L68" s="14">
+      <c r="L68" s="10">
         <v>15</v>
       </c>
-      <c r="M68" s="16">
+      <c r="M68" s="12">
         <v>12000</v>
       </c>
-      <c r="N68" s="16">
+      <c r="N68" s="12">
         <v>180000</v>
       </c>
-      <c r="O68" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P68" s="18" t="str">
+      <c r="O68" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P68" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A69" s="13">
+      <c r="A69" s="9">
         <v>45940</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C69" s="14" t="s">
+      <c r="C69" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D69" s="14" t="s">
+      <c r="D69" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E69" s="14" t="s">
+      <c r="E69" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F69" s="14">
+      <c r="F69" s="10">
         <v>768059355</v>
       </c>
-      <c r="G69" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H69" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I69" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J69" s="15" t="s">
+      <c r="G69" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H69" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I69" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J69" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K69" s="14" t="s">
+      <c r="K69" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="L69" s="14">
+      <c r="L69" s="10">
         <v>1</v>
       </c>
-      <c r="M69" s="16">
+      <c r="M69" s="12">
         <v>12500</v>
       </c>
-      <c r="N69" s="16">
+      <c r="N69" s="12">
         <v>12500</v>
       </c>
-      <c r="O69" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P69" s="18" t="str">
+      <c r="O69" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P69" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A70" s="13">
+      <c r="A70" s="9">
         <v>45940</v>
       </c>
-      <c r="B70" s="14" t="s">
+      <c r="B70" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C70" s="14" t="s">
+      <c r="C70" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D70" s="14" t="s">
+      <c r="D70" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E70" s="14" t="s">
+      <c r="E70" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F70" s="14">
+      <c r="F70" s="10">
         <v>768059355</v>
       </c>
-      <c r="G70" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H70" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I70" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J70" s="15" t="s">
+      <c r="G70" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H70" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I70" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J70" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K70" s="14" t="s">
+      <c r="K70" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="L70" s="14">
+      <c r="L70" s="10">
         <v>1</v>
       </c>
-      <c r="M70" s="16">
+      <c r="M70" s="12">
         <v>10000</v>
       </c>
-      <c r="N70" s="16">
+      <c r="N70" s="12">
         <v>10000</v>
       </c>
-      <c r="O70" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P70" s="18" t="str">
+      <c r="O70" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P70" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A71" s="13">
+      <c r="A71" s="9">
         <v>45940</v>
       </c>
-      <c r="B71" s="14" t="s">
+      <c r="B71" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C71" s="14" t="s">
+      <c r="C71" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D71" s="14" t="s">
+      <c r="D71" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E71" s="14" t="s">
+      <c r="E71" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F71" s="14">
+      <c r="F71" s="10">
         <v>768059355</v>
       </c>
-      <c r="G71" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H71" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I71" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J71" s="15" t="s">
+      <c r="G71" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H71" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I71" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J71" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K71" s="14" t="s">
+      <c r="K71" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L71" s="14">
+      <c r="L71" s="10">
         <v>30</v>
       </c>
-      <c r="M71" s="16">
-        <v>31000</v>
-      </c>
-      <c r="N71" s="16">
-        <v>930000</v>
-      </c>
-      <c r="O71" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P71" s="18" t="str">
+      <c r="M71" s="12">
+        <v>30500</v>
+      </c>
+      <c r="N71" s="12">
+        <v>915000</v>
+      </c>
+      <c r="O71" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P71" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A72" s="13">
+      <c r="A72" s="9">
         <v>45940</v>
       </c>
-      <c r="B72" s="14" t="s">
+      <c r="B72" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C72" s="14" t="s">
+      <c r="C72" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D72" s="14" t="s">
+      <c r="D72" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E72" s="14" t="s">
+      <c r="E72" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="F72" s="14">
+      <c r="F72" s="10">
         <v>774521295</v>
       </c>
-      <c r="G72" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H72" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I72" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J72" s="15" t="s">
+      <c r="G72" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H72" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J72" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K72" s="14" t="s">
+      <c r="K72" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L72" s="14">
+      <c r="L72" s="10">
         <v>25</v>
       </c>
-      <c r="M72" s="16">
+      <c r="M72" s="12">
         <v>26000</v>
       </c>
-      <c r="N72" s="16">
+      <c r="N72" s="12">
         <v>650000</v>
       </c>
-      <c r="O72" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P72" s="18" t="str">
+      <c r="O72" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P72" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A73" s="13">
+      <c r="A73" s="9">
         <v>45940</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B73" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C73" s="14" t="s">
+      <c r="C73" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D73" s="14" t="s">
+      <c r="D73" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E73" s="14" t="s">
+      <c r="E73" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="F73" s="14">
+      <c r="F73" s="10">
         <v>775586819</v>
       </c>
-      <c r="G73" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H73" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I73" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J73" s="15" t="s">
+      <c r="G73" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H73" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I73" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J73" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K73" s="14" t="s">
+      <c r="K73" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L73" s="14">
+      <c r="L73" s="10">
         <v>25</v>
       </c>
-      <c r="M73" s="16">
+      <c r="M73" s="12">
         <v>26000</v>
       </c>
-      <c r="N73" s="16">
+      <c r="N73" s="12">
         <v>650000</v>
       </c>
-      <c r="O73" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P73" s="18" t="str">
+      <c r="O73" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P73" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A74" s="13">
+      <c r="A74" s="9">
         <v>45940</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C74" s="14" t="s">
+      <c r="C74" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D74" s="14" t="s">
+      <c r="D74" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="E74" s="14" t="s">
+      <c r="E74" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="F74" s="14">
+      <c r="F74" s="10">
         <v>771207041</v>
       </c>
-      <c r="G74" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H74" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I74" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J74" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="K74" s="14" t="s">
+      <c r="G74" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H74" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I74" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J74" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K74" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L74" s="14">
+      <c r="L74" s="10">
         <v>25</v>
       </c>
-      <c r="M74" s="16">
+      <c r="M74" s="12">
         <v>26000</v>
       </c>
-      <c r="N74" s="16">
+      <c r="N74" s="12">
         <v>650000</v>
       </c>
-      <c r="O74" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P74" s="18" t="str">
+      <c r="O74" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P74" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A75" s="13">
+      <c r="A75" s="9">
         <v>45940</v>
       </c>
-      <c r="B75" s="14" t="s">
+      <c r="B75" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C75" s="14" t="s">
+      <c r="C75" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D75" s="14" t="s">
+      <c r="D75" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E75" s="14" t="s">
+      <c r="E75" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="F75" s="14">
+      <c r="F75" s="10">
         <v>781297575</v>
       </c>
-      <c r="G75" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H75" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I75" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J75" s="15" t="s">
+      <c r="G75" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H75" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I75" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J75" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K75" s="14" t="s">
+      <c r="K75" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L75" s="14">
+      <c r="L75" s="10">
         <v>25</v>
       </c>
-      <c r="M75" s="16">
+      <c r="M75" s="12">
         <v>26000</v>
       </c>
-      <c r="N75" s="16">
+      <c r="N75" s="12">
         <v>650000</v>
       </c>
-      <c r="O75" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P75" s="18" t="str">
+      <c r="O75" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P75" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A76" s="13">
+      <c r="A76" s="9">
         <v>45940</v>
       </c>
-      <c r="B76" s="14" t="s">
+      <c r="B76" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C76" s="14" t="s">
+      <c r="C76" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D76" s="14" t="s">
+      <c r="D76" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="E76" s="14" t="s">
+      <c r="E76" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="F76" s="14">
+      <c r="F76" s="10">
         <v>772252177</v>
       </c>
-      <c r="G76" s="14" t="s">
+      <c r="G76" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="H76" s="14" t="s">
+      <c r="H76" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="I76" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J76" s="15" t="s">
+      <c r="I76" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="K76" s="14" t="s">
+      <c r="K76" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L76" s="14">
+      <c r="L76" s="10">
         <v>25</v>
       </c>
-      <c r="M76" s="16">
+      <c r="M76" s="12">
         <v>26000</v>
       </c>
-      <c r="N76" s="16">
+      <c r="N76" s="12">
         <v>650000</v>
       </c>
-      <c r="O76" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P76" s="18" t="str">
+      <c r="O76" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P76" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A77" s="13">
+      <c r="A77" s="9">
         <v>45940</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C77" s="14" t="s">
+      <c r="C77" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D77" s="14" t="s">
+      <c r="D77" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="E77" s="14" t="s">
+      <c r="E77" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="F77" s="14">
+      <c r="F77" s="10">
         <v>785107921</v>
       </c>
-      <c r="G77" s="14" t="s">
+      <c r="G77" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="H77" s="14" t="s">
+      <c r="H77" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="I77" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J77" s="15" t="s">
+      <c r="I77" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J77" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="K77" s="14" t="s">
+      <c r="K77" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="L77" s="14">
+      <c r="L77" s="10">
         <v>25</v>
       </c>
-      <c r="M77" s="16">
+      <c r="M77" s="12">
         <v>11500</v>
       </c>
-      <c r="N77" s="16">
+      <c r="N77" s="12">
         <v>287500</v>
       </c>
-      <c r="O77" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P77" s="18" t="str">
+      <c r="O77" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P77" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A78" s="13">
+      <c r="A78" s="9">
         <v>45940</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B78" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C78" s="14" t="s">
+      <c r="C78" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D78" s="14" t="s">
+      <c r="D78" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="E78" s="14" t="s">
+      <c r="E78" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="F78" s="14">
+      <c r="F78" s="10">
         <v>772443935</v>
       </c>
-      <c r="G78" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H78" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I78" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J78" s="15" t="s">
+      <c r="G78" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H78" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I78" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J78" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="K78" s="14" t="s">
+      <c r="K78" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L78" s="14">
+      <c r="L78" s="10">
         <v>25</v>
       </c>
-      <c r="M78" s="16">
+      <c r="M78" s="12">
         <v>26000</v>
       </c>
-      <c r="N78" s="16">
+      <c r="N78" s="12">
         <v>650000</v>
       </c>
-      <c r="O78" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P78" s="18" t="str">
+      <c r="O78" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P78" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A79" s="13">
+      <c r="A79" s="9">
         <v>45939</v>
       </c>
-      <c r="B79" s="14" t="s">
+      <c r="B79" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C79" s="14" t="s">
+      <c r="C79" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D79" s="14" t="s">
+      <c r="D79" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="E79" s="14" t="s">
+      <c r="E79" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="F79" s="14">
+      <c r="F79" s="10">
         <v>772064446</v>
       </c>
-      <c r="G79" s="14" t="s">
+      <c r="G79" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="H79" s="14" t="s">
+      <c r="H79" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="I79" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J79" s="15" t="s">
+      <c r="I79" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J79" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="K79" s="14" t="s">
+      <c r="K79" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L79" s="14">
+      <c r="L79" s="10">
         <v>25</v>
       </c>
-      <c r="M79" s="16">
+      <c r="M79" s="12">
         <v>19500</v>
       </c>
-      <c r="N79" s="16">
+      <c r="N79" s="12">
         <v>487500</v>
       </c>
-      <c r="O79" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P79" s="18" t="str">
+      <c r="O79" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P79" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A80" s="13">
+      <c r="A80" s="9">
         <v>45939</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B80" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="14" t="s">
+      <c r="C80" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D80" s="14" t="s">
+      <c r="D80" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="E80" s="14" t="s">
+      <c r="E80" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="F80" s="14">
+      <c r="F80" s="10">
         <v>775411988</v>
       </c>
-      <c r="G80" s="14" t="s">
+      <c r="G80" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="H80" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I80" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J80" s="15" t="s">
+      <c r="H80" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I80" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J80" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="K80" s="14" t="s">
+      <c r="K80" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="L80" s="14">
+      <c r="L80" s="10">
         <v>25</v>
       </c>
-      <c r="M80" s="16">
+      <c r="M80" s="12">
         <v>12500</v>
       </c>
-      <c r="N80" s="16">
+      <c r="N80" s="12">
         <v>312500</v>
       </c>
-      <c r="O80" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P80" s="18" t="str">
+      <c r="O80" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P80" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A81" s="13">
+      <c r="A81" s="9">
         <v>45939</v>
       </c>
-      <c r="B81" s="14" t="s">
+      <c r="B81" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C81" s="14" t="s">
+      <c r="C81" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D81" s="14" t="s">
+      <c r="D81" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="E81" s="14" t="s">
+      <c r="E81" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="F81" s="14">
+      <c r="F81" s="10">
         <v>775411988</v>
       </c>
-      <c r="G81" s="14" t="s">
+      <c r="G81" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="H81" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I81" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J81" s="15" t="s">
+      <c r="H81" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I81" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J81" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="K81" s="14" t="s">
+      <c r="K81" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L81" s="14">
+      <c r="L81" s="10">
         <v>5</v>
       </c>
-      <c r="M81" s="16">
+      <c r="M81" s="12">
         <v>19500</v>
       </c>
-      <c r="N81" s="16">
+      <c r="N81" s="12">
         <v>97500</v>
       </c>
-      <c r="O81" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P81" s="18" t="str">
+      <c r="O81" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P81" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A82" s="13">
+      <c r="A82" s="9">
         <v>45939</v>
       </c>
-      <c r="B82" s="14" t="s">
+      <c r="B82" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C82" s="14" t="s">
+      <c r="C82" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D82" s="14" t="s">
+      <c r="D82" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E82" s="14" t="s">
+      <c r="E82" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F82" s="14">
+      <c r="F82" s="10">
         <v>775602981</v>
       </c>
-      <c r="G82" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H82" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I82" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J82" s="15" t="s">
+      <c r="G82" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H82" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I82" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J82" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="K82" s="14" t="s">
+      <c r="K82" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="L82" s="14">
+      <c r="L82" s="10">
         <v>25</v>
       </c>
-      <c r="M82" s="16">
+      <c r="M82" s="12">
         <v>12500</v>
       </c>
-      <c r="N82" s="16">
+      <c r="N82" s="12">
         <v>312500</v>
       </c>
-      <c r="O82" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P82" s="18" t="str">
+      <c r="O82" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P82" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A83" s="13">
+      <c r="A83" s="9">
         <v>45939</v>
       </c>
-      <c r="B83" s="14" t="s">
+      <c r="B83" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C83" s="14" t="s">
+      <c r="C83" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D83" s="14" t="s">
+      <c r="D83" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E83" s="14" t="s">
+      <c r="E83" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F83" s="14">
+      <c r="F83" s="10">
         <v>775602981</v>
       </c>
-      <c r="G83" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H83" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I83" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J83" s="15" t="s">
+      <c r="G83" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H83" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I83" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J83" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="K83" s="14" t="s">
+      <c r="K83" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="L83" s="14">
+      <c r="L83" s="10">
         <v>4</v>
       </c>
-      <c r="M83" s="16">
+      <c r="M83" s="12">
         <v>10000</v>
       </c>
-      <c r="N83" s="16">
+      <c r="N83" s="12">
         <v>40000</v>
       </c>
-      <c r="O83" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P83" s="18" t="str">
+      <c r="O83" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P83" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A84" s="13">
+      <c r="A84" s="9">
         <v>45939</v>
       </c>
-      <c r="B84" s="14" t="s">
+      <c r="B84" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C84" s="14" t="s">
+      <c r="C84" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D84" s="14" t="s">
+      <c r="D84" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="E84" s="14" t="s">
+      <c r="E84" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="F84" s="14">
+      <c r="F84" s="10">
         <v>775276149</v>
       </c>
-      <c r="G84" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H84" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I84" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J84" s="15" t="s">
+      <c r="G84" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H84" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I84" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J84" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="K84" s="14" t="s">
+      <c r="K84" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="L84" s="14">
+      <c r="L84" s="10">
         <v>5</v>
       </c>
-      <c r="M84" s="16">
+      <c r="M84" s="12">
         <v>12500</v>
       </c>
-      <c r="N84" s="16">
+      <c r="N84" s="12">
         <v>62500</v>
       </c>
-      <c r="O84" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P84" s="18" t="str">
+      <c r="O84" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P84" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A85" s="13">
+      <c r="A85" s="9">
         <v>45939</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B85" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C85" s="14" t="s">
+      <c r="C85" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D85" s="14" t="s">
+      <c r="D85" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="E85" s="14" t="s">
+      <c r="E85" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="F85" s="14">
+      <c r="F85" s="10">
         <v>775276149</v>
       </c>
-      <c r="G85" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H85" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I85" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J85" s="15" t="s">
+      <c r="G85" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H85" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I85" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J85" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="K85" s="14" t="s">
+      <c r="K85" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="L85" s="14">
+      <c r="L85" s="10">
         <v>3</v>
       </c>
-      <c r="M85" s="16">
+      <c r="M85" s="12">
         <v>10000</v>
       </c>
-      <c r="N85" s="16">
+      <c r="N85" s="12">
         <v>30000</v>
       </c>
-      <c r="O85" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P85" s="18" t="str">
+      <c r="O85" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P85" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A86" s="13">
+      <c r="A86" s="9">
         <v>45939</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B86" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C86" s="14" t="s">
+      <c r="C86" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D86" s="14" t="s">
+      <c r="D86" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E86" s="14" t="s">
+      <c r="E86" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="F86" s="14">
+      <c r="F86" s="10">
         <v>781297575</v>
       </c>
-      <c r="G86" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H86" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I86" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J86" s="15" t="s">
+      <c r="G86" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H86" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I86" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J86" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K86" s="14" t="s">
+      <c r="K86" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L86" s="14">
+      <c r="L86" s="10">
         <v>25</v>
       </c>
-      <c r="M86" s="16">
+      <c r="M86" s="12">
         <v>19500</v>
       </c>
-      <c r="N86" s="16">
+      <c r="N86" s="12">
         <v>487500</v>
       </c>
-      <c r="O86" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P86" s="18" t="str">
+      <c r="O86" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P86" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A87" s="13">
+      <c r="A87" s="9">
         <v>45939</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B87" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C87" s="14" t="s">
+      <c r="C87" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D87" s="14" t="s">
+      <c r="D87" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E87" s="14" t="s">
+      <c r="E87" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F87" s="14">
+      <c r="F87" s="10">
         <v>774216339</v>
       </c>
-      <c r="G87" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H87" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I87" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J87" s="15" t="s">
+      <c r="G87" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H87" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I87" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J87" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K87" s="14" t="s">
+      <c r="K87" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="L87" s="14">
+      <c r="L87" s="10">
         <v>25</v>
       </c>
-      <c r="M87" s="16">
+      <c r="M87" s="12">
         <v>9750</v>
       </c>
-      <c r="N87" s="16">
+      <c r="N87" s="12">
         <v>243750</v>
       </c>
-      <c r="O87" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P87" s="18" t="str">
+      <c r="O87" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P87" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A88" s="13">
+      <c r="A88" s="9">
         <v>45939</v>
       </c>
-      <c r="B88" s="14" t="s">
+      <c r="B88" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C88" s="14" t="s">
+      <c r="C88" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D88" s="14" t="s">
+      <c r="D88" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E88" s="14" t="s">
+      <c r="E88" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="F88" s="14">
+      <c r="F88" s="10">
         <v>774880562</v>
       </c>
-      <c r="G88" s="14" t="s">
+      <c r="G88" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="H88" s="14" t="s">
+      <c r="H88" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="I88" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J88" s="15" t="s">
+      <c r="I88" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J88" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K88" s="14" t="s">
+      <c r="K88" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="L88" s="14">
+      <c r="L88" s="10">
         <v>8</v>
       </c>
-      <c r="M88" s="16">
+      <c r="M88" s="12">
         <v>15500</v>
       </c>
-      <c r="N88" s="16">
+      <c r="N88" s="12">
         <v>124000</v>
       </c>
-      <c r="O88" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P88" s="18" t="str">
+      <c r="O88" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P88" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A89" s="13">
+      <c r="A89" s="9">
         <v>45939</v>
       </c>
-      <c r="B89" s="14" t="s">
+      <c r="B89" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C89" s="14" t="s">
+      <c r="C89" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D89" s="14" t="s">
+      <c r="D89" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E89" s="14" t="s">
+      <c r="E89" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="F89" s="14">
+      <c r="F89" s="10">
         <v>705121758</v>
       </c>
-      <c r="G89" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H89" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I89" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J89" s="15" t="s">
+      <c r="G89" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H89" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I89" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J89" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K89" s="14" t="s">
+      <c r="K89" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="L89" s="14">
+      <c r="L89" s="10">
         <v>7</v>
       </c>
-      <c r="M89" s="16">
+      <c r="M89" s="12">
         <v>12500</v>
       </c>
-      <c r="N89" s="16">
+      <c r="N89" s="12">
         <v>87500</v>
       </c>
-      <c r="O89" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P89" s="18" t="str">
+      <c r="O89" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P89" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A90" s="13">
+      <c r="A90" s="9">
         <v>45939</v>
       </c>
-      <c r="B90" s="14" t="s">
+      <c r="B90" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C90" s="14" t="s">
+      <c r="C90" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D90" s="14" t="s">
+      <c r="D90" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E90" s="14" t="s">
+      <c r="E90" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="F90" s="14">
+      <c r="F90" s="10">
         <v>705121758</v>
       </c>
-      <c r="G90" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H90" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I90" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J90" s="15" t="s">
+      <c r="G90" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H90" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I90" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J90" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K90" s="14" t="s">
+      <c r="K90" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="L90" s="14">
+      <c r="L90" s="10">
         <v>50</v>
       </c>
-      <c r="M90" s="16">
+      <c r="M90" s="12">
         <v>11500</v>
       </c>
-      <c r="N90" s="16">
+      <c r="N90" s="12">
         <v>575000</v>
       </c>
-      <c r="O90" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P90" s="18" t="str">
+      <c r="O90" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P90" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A91" s="13">
+      <c r="A91" s="9">
         <v>45939</v>
       </c>
-      <c r="B91" s="14" t="s">
+      <c r="B91" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C91" s="14" t="s">
+      <c r="C91" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D91" s="14" t="s">
+      <c r="D91" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="E91" s="14" t="s">
+      <c r="E91" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="F91" s="14">
+      <c r="F91" s="10">
         <v>775276149</v>
       </c>
-      <c r="G91" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H91" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I91" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J91" s="15" t="s">
+      <c r="G91" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H91" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I91" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J91" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="K91" s="14" t="s">
+      <c r="K91" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="L91" s="14">
+      <c r="L91" s="10">
         <v>5</v>
       </c>
-      <c r="M91" s="16">
+      <c r="M91" s="12">
         <v>15500</v>
       </c>
-      <c r="N91" s="16">
+      <c r="N91" s="12">
         <v>77500</v>
       </c>
-      <c r="O91" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P91" s="18" t="str">
+      <c r="O91" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P91" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A92" s="13">
+      <c r="A92" s="9">
         <v>45939</v>
       </c>
-      <c r="B92" s="14" t="s">
+      <c r="B92" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C92" s="14" t="s">
+      <c r="C92" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D92" s="14" t="s">
+      <c r="D92" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="E92" s="14" t="s">
+      <c r="E92" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="F92" s="14">
+      <c r="F92" s="10">
         <v>775276149</v>
       </c>
-      <c r="G92" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H92" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I92" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J92" s="15" t="s">
+      <c r="G92" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H92" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I92" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J92" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="K92" s="14" t="s">
+      <c r="K92" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="L92" s="14">
+      <c r="L92" s="10">
         <v>11</v>
       </c>
-      <c r="M92" s="16">
+      <c r="M92" s="12">
         <v>12000</v>
       </c>
-      <c r="N92" s="16">
+      <c r="N92" s="12">
         <v>132000</v>
       </c>
-      <c r="O92" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P92" s="18" t="str">
+      <c r="O92" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P92" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A93" s="13">
+      <c r="A93" s="9">
         <v>45939</v>
       </c>
-      <c r="B93" s="14" t="s">
+      <c r="B93" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C93" s="14" t="s">
+      <c r="C93" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D93" s="14" t="s">
+      <c r="D93" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="E93" s="14" t="s">
+      <c r="E93" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="F93" s="14">
+      <c r="F93" s="10">
         <v>775276149</v>
       </c>
-      <c r="G93" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H93" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I93" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J93" s="15" t="s">
+      <c r="G93" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H93" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I93" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J93" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="K93" s="14" t="s">
+      <c r="K93" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="L93" s="14">
+      <c r="L93" s="10">
         <v>10</v>
       </c>
-      <c r="M93" s="16">
+      <c r="M93" s="12">
         <v>7500</v>
       </c>
-      <c r="N93" s="16">
+      <c r="N93" s="12">
         <v>75000</v>
       </c>
-      <c r="O93" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P93" s="18" t="str">
+      <c r="O93" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P93" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A94" s="13">
+      <c r="A94" s="9">
         <v>45939</v>
       </c>
-      <c r="B94" s="14" t="s">
+      <c r="B94" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C94" s="14" t="s">
+      <c r="C94" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D94" s="14" t="s">
+      <c r="D94" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="E94" s="14" t="s">
+      <c r="E94" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="F94" s="14">
+      <c r="F94" s="10">
         <v>775276149</v>
       </c>
-      <c r="G94" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H94" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I94" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J94" s="15" t="s">
+      <c r="G94" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H94" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I94" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J94" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="K94" s="14" t="s">
+      <c r="K94" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L94" s="14">
+      <c r="L94" s="10">
         <v>25</v>
       </c>
-      <c r="M94" s="16">
+      <c r="M94" s="12">
         <v>26000</v>
       </c>
-      <c r="N94" s="16">
+      <c r="N94" s="12">
         <v>650000</v>
       </c>
-      <c r="O94" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P94" s="18" t="str">
+      <c r="O94" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P94" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A95" s="13">
+      <c r="A95" s="9">
         <v>45939</v>
       </c>
-      <c r="B95" s="14" t="s">
+      <c r="B95" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C95" s="14" t="s">
+      <c r="C95" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D95" s="14" t="s">
+      <c r="D95" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="E95" s="14" t="s">
+      <c r="E95" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="F95" s="14">
+      <c r="F95" s="10">
         <v>776194586</v>
       </c>
-      <c r="G95" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H95" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I95" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J95" s="15" t="s">
+      <c r="G95" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H95" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I95" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J95" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="K95" s="14" t="s">
+      <c r="K95" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L95" s="14">
+      <c r="L95" s="10">
         <v>25</v>
       </c>
-      <c r="M95" s="16">
+      <c r="M95" s="12">
         <v>26000</v>
       </c>
-      <c r="N95" s="16">
+      <c r="N95" s="12">
         <v>650000</v>
       </c>
-      <c r="O95" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P95" s="18" t="str">
+      <c r="O95" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P95" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A96" s="13">
+      <c r="A96" s="9">
         <v>45939</v>
       </c>
-      <c r="B96" s="14" t="s">
+      <c r="B96" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C96" s="14" t="s">
+      <c r="C96" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D96" s="14" t="s">
+      <c r="D96" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E96" s="14" t="s">
+      <c r="E96" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="F96" s="14">
+      <c r="F96" s="10">
         <v>786323232</v>
       </c>
-      <c r="G96" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H96" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I96" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J96" s="15" t="s">
+      <c r="G96" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H96" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I96" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J96" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K96" s="14" t="s">
+      <c r="K96" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L96" s="14">
+      <c r="L96" s="10">
         <v>100</v>
       </c>
-      <c r="M96" s="16">
+      <c r="M96" s="12">
         <v>26000</v>
       </c>
-      <c r="N96" s="16">
+      <c r="N96" s="12">
         <v>2600000</v>
       </c>
-      <c r="O96" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P96" s="18" t="str">
+      <c r="O96" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P96" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A97" s="13">
+      <c r="A97" s="9">
         <v>45939</v>
       </c>
-      <c r="B97" s="14" t="s">
+      <c r="B97" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C97" s="14" t="s">
+      <c r="C97" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D97" s="14" t="s">
+      <c r="D97" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E97" s="14" t="s">
+      <c r="E97" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F97" s="14">
+      <c r="F97" s="10">
         <v>783758073</v>
       </c>
-      <c r="G97" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H97" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I97" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J97" s="15" t="s">
+      <c r="G97" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H97" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I97" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J97" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="K97" s="14" t="s">
+      <c r="K97" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="L97" s="14">
+      <c r="L97" s="10">
         <v>25</v>
       </c>
-      <c r="M97" s="16">
+      <c r="M97" s="12">
         <v>9750</v>
       </c>
-      <c r="N97" s="16">
+      <c r="N97" s="12">
         <v>243750</v>
       </c>
-      <c r="O97" s="17" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S41</v>
-      </c>
-      <c r="P97" s="18" t="str">
+      <c r="O97" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S41</v>
+      </c>
+      <c r="P97" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>

</xml_diff>

<commit_message>
Rapport du 18 Octobre 2025
</commit_message>
<xml_diff>
--- a/Donnees_RZ.xlsx
+++ b/Donnees_RZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCBD103-D7EC-4112-A13F-7A9D447F0261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D725AA2F-DCB8-4646-98B3-358FCAB47CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="129">
   <si>
     <t>Date</t>
   </si>
@@ -330,6 +330,96 @@
   </si>
   <si>
     <t>Il avait commandé le stick et les pots 50 et 200g mais il a fini par acheter d'autres pots</t>
+  </si>
+  <si>
+    <t>Terminus 54</t>
+  </si>
+  <si>
+    <t>Abdourahmane</t>
+  </si>
+  <si>
+    <t>PA DIOP</t>
+  </si>
+  <si>
+    <t>SALIOU BA</t>
+  </si>
+  <si>
+    <t>Ndiaye Malika</t>
+  </si>
+  <si>
+    <t>Seynabou SOW</t>
+  </si>
+  <si>
+    <t>CASTOR</t>
+  </si>
+  <si>
+    <t>Castor</t>
+  </si>
+  <si>
+    <t>Alioune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depuis lundi jusqu'à présent </t>
+  </si>
+  <si>
+    <t>Ben Tally</t>
+  </si>
+  <si>
+    <t>El Hadji</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merci beaucoup </t>
+  </si>
+  <si>
+    <t>Liberté 1 à 6</t>
+  </si>
+  <si>
+    <t>Omar</t>
+  </si>
+  <si>
+    <t>Ces lan</t>
+  </si>
+  <si>
+    <t>Pape</t>
+  </si>
+  <si>
+    <t>Pape castor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sa prend du temps </t>
+  </si>
+  <si>
+    <t>Mame cheikh</t>
+  </si>
+  <si>
+    <t>Assane Wade</t>
+  </si>
+  <si>
+    <t>Café stick Altimo 1,5gx09boites</t>
+  </si>
+  <si>
+    <t>Diamaguene</t>
+  </si>
+  <si>
+    <t>Korka</t>
+  </si>
+  <si>
+    <t>Mamadou DIBA</t>
+  </si>
+  <si>
+    <t>Supermarché</t>
+  </si>
+  <si>
+    <t>Alassane</t>
+  </si>
+  <si>
+    <t>Merci beaucoup</t>
+  </si>
+  <si>
+    <t>Café Altimo pot 100g x 24 pcs</t>
+  </si>
+  <si>
+    <t>Café Altimo pot 200g x 12 pcs</t>
   </si>
 </sst>
 </file>
@@ -720,8 +810,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P43" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A1:P43" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P59" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A1:P59" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{F85C405C-E78B-4DA6-8568-08107D7551E4}" name="Date" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{24A95AD6-D6B8-4864-9451-50BFB3565C62}" name="Prenom_Nom_RZ" dataDxfId="15"/>
@@ -1034,10 +1124,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:P59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1267,7 +1357,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" s="11">
-        <v>45946</v>
+        <v>45947</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>52</v>
@@ -1276,19 +1366,19 @@
         <v>53</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="F5" s="12">
-        <v>771987678</v>
+        <v>771701320</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>17</v>
@@ -1297,16 +1387,16 @@
         <v>64</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="L5" s="12">
         <v>25</v>
       </c>
       <c r="M5" s="14">
-        <v>11500</v>
+        <v>9750</v>
       </c>
       <c r="N5" s="14">
-        <v>287500</v>
+        <v>243750</v>
       </c>
       <c r="O5" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -1319,22 +1409,22 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" s="11">
-        <v>45946</v>
+        <v>45947</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="F6" s="12">
-        <v>776212473</v>
+        <v>764881522</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>47</v>
@@ -1346,19 +1436,19 @@
         <v>17</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>21</v>
       </c>
       <c r="L6" s="12">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="M6" s="14">
-        <v>18750</v>
+        <v>19500</v>
       </c>
       <c r="N6" s="14">
-        <v>243750</v>
+        <v>97500</v>
       </c>
       <c r="O6" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -1371,25 +1461,25 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" s="11">
-        <v>45946</v>
+        <v>45947</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="F7" s="12">
-        <v>784426640</v>
+        <v>772884203</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>13</v>
@@ -1398,19 +1488,19 @@
         <v>17</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="L7" s="12">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="M7" s="14">
-        <v>11500</v>
+        <v>19500</v>
       </c>
       <c r="N7" s="14">
-        <v>287500</v>
+        <v>97500</v>
       </c>
       <c r="O7" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -1423,46 +1513,46 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" s="11">
-        <v>45946</v>
+        <v>45947</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="F8" s="12">
-        <v>773340367</v>
+        <v>772494182</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>47</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>17</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="L8" s="12">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="M8" s="14">
-        <v>19500</v>
+        <v>9750</v>
       </c>
       <c r="N8" s="14">
-        <v>234000</v>
+        <v>48750</v>
       </c>
       <c r="O8" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -1475,46 +1565,46 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" s="11">
-        <v>45946</v>
+        <v>45947</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>15</v>
+        <v>105</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="F9" s="12">
-        <v>775411988</v>
+        <v>775538380</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="I9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="L9" s="12">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="M9" s="14">
-        <v>15500</v>
+        <v>19500</v>
       </c>
       <c r="N9" s="14">
-        <v>387500</v>
+        <v>19500</v>
       </c>
       <c r="O9" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -1527,46 +1617,46 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" s="11">
-        <v>45945</v>
+        <v>45947</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="F10" s="12">
-        <v>775273147</v>
+        <v>775987400</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>17</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="L10" s="12">
         <v>1</v>
       </c>
       <c r="M10" s="14">
-        <v>10000</v>
+        <v>19500</v>
       </c>
       <c r="N10" s="14">
-        <v>10000</v>
+        <v>19500</v>
       </c>
       <c r="O10" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -1579,25 +1669,25 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" s="11">
-        <v>45945</v>
+        <v>45947</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>32</v>
+        <v>113</v>
       </c>
       <c r="F11" s="12">
-        <v>775273147</v>
+        <v>773170826</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>13</v>
@@ -1606,19 +1696,19 @@
         <v>17</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="L11" s="12">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="M11" s="14">
-        <v>6000</v>
+        <v>19500</v>
       </c>
       <c r="N11" s="14">
-        <v>150000</v>
+        <v>39000</v>
       </c>
       <c r="O11" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -1631,46 +1721,46 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" s="11">
-        <v>45945</v>
+        <v>45947</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>32</v>
+        <v>115</v>
       </c>
       <c r="F12" s="12">
-        <v>775273147</v>
+        <v>777972938</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="I12" s="12" t="s">
         <v>17</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="L12" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M12" s="14">
-        <v>26000</v>
+        <v>12500</v>
       </c>
       <c r="N12" s="14">
-        <v>52000</v>
+        <v>12500</v>
       </c>
       <c r="O12" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -1683,46 +1773,46 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" s="11">
-        <v>45945</v>
+        <v>45947</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="F13" s="12">
-        <v>775273147</v>
+        <v>772900705</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>16</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="I13" s="12" t="s">
         <v>17</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="L13" s="12">
         <v>1</v>
       </c>
       <c r="M13" s="14">
-        <v>12500</v>
+        <v>26000</v>
       </c>
       <c r="N13" s="14">
-        <v>12500</v>
+        <v>26000</v>
       </c>
       <c r="O13" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -1735,22 +1825,22 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" s="11">
-        <v>45945</v>
+        <v>45947</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="F14" s="12">
-        <v>767379110</v>
+        <v>776167544</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>16</v>
@@ -1762,19 +1852,19 @@
         <v>17</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="L14" s="12">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M14" s="14">
-        <v>15500</v>
+        <v>11500</v>
       </c>
       <c r="N14" s="14">
-        <v>108500</v>
+        <v>23000</v>
       </c>
       <c r="O14" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -1787,25 +1877,25 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" s="11">
-        <v>45945</v>
+        <v>45947</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
       <c r="F15" s="12">
-        <v>763469670</v>
+        <v>775884054</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>13</v>
@@ -1814,19 +1904,19 @@
         <v>17</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="L15" s="12">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="M15" s="14">
-        <v>26000</v>
+        <v>31000</v>
       </c>
       <c r="N15" s="14">
-        <v>2600000</v>
+        <v>31000</v>
       </c>
       <c r="O15" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -1839,25 +1929,25 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" s="11">
-        <v>45945</v>
+        <v>45947</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="F16" s="12">
-        <v>781757464</v>
+        <v>772131614</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>13</v>
@@ -1866,19 +1956,19 @@
         <v>17</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L16" s="12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M16" s="14">
-        <v>19500</v>
+        <v>26000</v>
       </c>
       <c r="N16" s="14">
-        <v>97500</v>
+        <v>26000</v>
       </c>
       <c r="O16" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -1891,25 +1981,25 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17" s="11">
-        <v>45945</v>
+        <v>45947</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>44</v>
+        <v>121</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="F17" s="12">
-        <v>774540865</v>
+        <v>774446616</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>16</v>
+        <v>124</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>13</v>
@@ -1918,19 +2008,19 @@
         <v>17</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>25</v>
+        <v>111</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L17" s="12">
         <v>1</v>
       </c>
       <c r="M17" s="14">
-        <v>12500</v>
+        <v>15500</v>
       </c>
       <c r="N17" s="14">
-        <v>12500</v>
+        <v>15500</v>
       </c>
       <c r="O17" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -1943,7 +2033,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A18" s="11">
-        <v>45945</v>
+        <v>45946</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>52</v>
@@ -1952,37 +2042,37 @@
         <v>53</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="F18" s="12">
-        <v>771010134</v>
+        <v>771987678</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="I18" s="12" t="s">
         <v>17</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="L18" s="12">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="M18" s="14">
-        <v>26000</v>
+        <v>11500</v>
       </c>
       <c r="N18" s="14">
-        <v>2600000</v>
+        <v>287500</v>
       </c>
       <c r="O18" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -1995,7 +2085,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19" s="11">
-        <v>45945</v>
+        <v>45946</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>52</v>
@@ -2004,13 +2094,13 @@
         <v>53</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="F19" s="12">
-        <v>771010134</v>
+        <v>776212473</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>47</v>
@@ -2022,19 +2112,19 @@
         <v>17</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="L19" s="12">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="M19" s="14">
-        <v>10000</v>
+        <v>18750</v>
       </c>
       <c r="N19" s="14">
-        <v>10000</v>
+        <v>243750</v>
       </c>
       <c r="O19" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2047,7 +2137,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20" s="11">
-        <v>45945</v>
+        <v>45946</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>52</v>
@@ -2056,16 +2146,16 @@
         <v>53</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F20" s="12">
-        <v>771010134</v>
+        <v>784426640</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>13</v>
@@ -2074,19 +2164,19 @@
         <v>17</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="L20" s="12">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="M20" s="14">
-        <v>15500</v>
+        <v>11500</v>
       </c>
       <c r="N20" s="14">
-        <v>15500</v>
+        <v>287500</v>
       </c>
       <c r="O20" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2099,22 +2189,22 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21" s="11">
-        <v>45945</v>
+        <v>45946</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F21" s="12">
-        <v>771010134</v>
+        <v>773340367</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>47</v>
@@ -2126,19 +2216,19 @@
         <v>17</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="L21" s="12">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="M21" s="14">
-        <v>12500</v>
+        <v>19500</v>
       </c>
       <c r="N21" s="14">
-        <v>12500</v>
+        <v>234000</v>
       </c>
       <c r="O21" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2151,22 +2241,22 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22" s="11">
-        <v>45945</v>
+        <v>45946</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="F22" s="12">
-        <v>786323232</v>
+        <v>775894235</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>16</v>
@@ -2178,19 +2268,19 @@
         <v>17</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>21</v>
       </c>
       <c r="L22" s="12">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="M22" s="14">
-        <v>26000</v>
+        <v>19500</v>
       </c>
       <c r="N22" s="14">
-        <v>650000</v>
+        <v>19500</v>
       </c>
       <c r="O22" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2203,22 +2293,22 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" s="11">
-        <v>45945</v>
+        <v>45946</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="F23" s="12">
-        <v>784537895</v>
+        <v>775894235</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>16</v>
@@ -2230,19 +2320,19 @@
         <v>17</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>50</v>
+        <v>127</v>
       </c>
       <c r="L23" s="12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M23" s="14">
-        <v>15500</v>
+        <v>33500</v>
       </c>
       <c r="N23" s="14">
-        <v>15500</v>
+        <v>167500</v>
       </c>
       <c r="O23" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2255,22 +2345,22 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="11">
-        <v>45945</v>
+        <v>45946</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="F24" s="12">
-        <v>784537895</v>
+        <v>775894235</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>16</v>
@@ -2282,19 +2372,19 @@
         <v>17</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>49</v>
+        <v>128</v>
       </c>
       <c r="L24" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M24" s="14">
-        <v>12500</v>
+        <v>34500</v>
       </c>
       <c r="N24" s="14">
-        <v>12500</v>
+        <v>138000</v>
       </c>
       <c r="O24" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2307,25 +2397,25 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" s="11">
-        <v>45945</v>
+        <v>45946</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="F25" s="12">
-        <v>775541532</v>
+        <v>775411988</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>13</v>
@@ -2334,19 +2424,19 @@
         <v>17</v>
       </c>
       <c r="J25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L25" s="12">
         <v>25</v>
       </c>
-      <c r="K25" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="L25" s="12">
-        <v>10</v>
-      </c>
       <c r="M25" s="14">
-        <v>9750</v>
+        <v>15500</v>
       </c>
       <c r="N25" s="14">
-        <v>97500</v>
+        <v>387500</v>
       </c>
       <c r="O25" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2362,19 +2452,19 @@
         <v>45945</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="F26" s="12">
-        <v>774540865</v>
+        <v>775273147</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>16</v>
@@ -2386,19 +2476,19 @@
         <v>17</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L26" s="12">
         <v>1</v>
       </c>
       <c r="M26" s="14">
-        <v>15500</v>
+        <v>12500</v>
       </c>
       <c r="N26" s="14">
-        <v>15500</v>
+        <v>12500</v>
       </c>
       <c r="O26" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2414,19 +2504,19 @@
         <v>45945</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="F27" s="12">
-        <v>775405469</v>
+        <v>775273147</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>16</v>
@@ -2438,19 +2528,19 @@
         <v>17</v>
       </c>
       <c r="J27" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L27" s="12">
         <v>25</v>
       </c>
-      <c r="K27" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L27" s="12">
-        <v>5</v>
-      </c>
       <c r="M27" s="14">
-        <v>19500</v>
+        <v>6000</v>
       </c>
       <c r="N27" s="14">
-        <v>97500</v>
+        <v>150000</v>
       </c>
       <c r="O27" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2466,19 +2556,19 @@
         <v>45945</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F28" s="12">
-        <v>774245132</v>
+        <v>775273147</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>16</v>
@@ -2490,19 +2580,19 @@
         <v>17</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L28" s="12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M28" s="14">
-        <v>19500</v>
+        <v>26000</v>
       </c>
       <c r="N28" s="14">
-        <v>97500</v>
+        <v>52000</v>
       </c>
       <c r="O28" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2518,19 +2608,19 @@
         <v>45945</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="F29" s="12">
-        <v>771428937</v>
+        <v>775273147</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>16</v>
@@ -2542,19 +2632,19 @@
         <v>17</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="L29" s="12">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="M29" s="14">
-        <v>26000</v>
+        <v>10000</v>
       </c>
       <c r="N29" s="14">
-        <v>650000</v>
+        <v>10000</v>
       </c>
       <c r="O29" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2570,22 +2660,22 @@
         <v>45945</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="F30" s="12">
-        <v>785554540</v>
+        <v>767379110</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>13</v>
@@ -2594,19 +2684,19 @@
         <v>17</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="K30" s="12" t="s">
         <v>50</v>
       </c>
       <c r="L30" s="12">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M30" s="14">
         <v>15500</v>
       </c>
       <c r="N30" s="14">
-        <v>15500</v>
+        <v>108500</v>
       </c>
       <c r="O30" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2622,19 +2712,19 @@
         <v>45945</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F31" s="12">
-        <v>773756258</v>
+        <v>763469670</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>16</v>
@@ -2646,19 +2736,19 @@
         <v>17</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L31" s="12">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="M31" s="14">
-        <v>19500</v>
+        <v>26000</v>
       </c>
       <c r="N31" s="14">
-        <v>97500</v>
+        <v>2600000</v>
       </c>
       <c r="O31" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2674,22 +2764,22 @@
         <v>45945</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>83</v>
+        <v>31</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F32" s="12">
-        <v>773777037</v>
+        <v>781757464</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="H32" s="12" t="s">
         <v>13</v>
@@ -2698,19 +2788,19 @@
         <v>17</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="K32" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L32" s="12">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="M32" s="14">
-        <v>26000</v>
+        <v>19500</v>
       </c>
       <c r="N32" s="14">
-        <v>650000</v>
+        <v>97500</v>
       </c>
       <c r="O32" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2732,16 +2822,16 @@
         <v>19</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F33" s="12">
-        <v>773750007</v>
+        <v>774540865</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>86</v>
+        <v>16</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>13</v>
@@ -2753,16 +2843,16 @@
         <v>25</v>
       </c>
       <c r="K33" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L33" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M33" s="14">
-        <v>15500</v>
+        <v>12500</v>
       </c>
       <c r="N33" s="14">
-        <v>31000</v>
+        <v>12500</v>
       </c>
       <c r="O33" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2778,22 +2868,22 @@
         <v>45945</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F34" s="12">
-        <v>773750007</v>
+        <v>771010134</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>13</v>
@@ -2802,19 +2892,19 @@
         <v>17</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="L34" s="12">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="M34" s="14">
-        <v>15500</v>
+        <v>26000</v>
       </c>
       <c r="N34" s="14">
-        <v>15500</v>
+        <v>2600000</v>
       </c>
       <c r="O34" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2830,22 +2920,22 @@
         <v>45945</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F35" s="12">
-        <v>775171537</v>
+        <v>771010134</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="H35" s="12" t="s">
         <v>13</v>
@@ -2854,19 +2944,19 @@
         <v>17</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="K35" s="12" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="L35" s="12">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="M35" s="14">
-        <v>26000</v>
+        <v>10000</v>
       </c>
       <c r="N35" s="14">
-        <v>650000</v>
+        <v>10000</v>
       </c>
       <c r="O35" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2882,19 +2972,19 @@
         <v>45945</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="F36" s="12">
-        <v>776818022</v>
+        <v>771010134</v>
       </c>
       <c r="G36" s="12" t="s">
         <v>47</v>
@@ -2906,19 +2996,19 @@
         <v>17</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="L36" s="12">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="M36" s="14">
-        <v>9750</v>
+        <v>15500</v>
       </c>
       <c r="N36" s="14">
-        <v>243750</v>
+        <v>15500</v>
       </c>
       <c r="O36" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2934,22 +3024,22 @@
         <v>45945</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F37" s="12">
-        <v>773199049</v>
+        <v>771010134</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="H37" s="12" t="s">
         <v>13</v>
@@ -2958,19 +3048,19 @@
         <v>17</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="L37" s="12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M37" s="14">
-        <v>10000</v>
+        <v>12500</v>
       </c>
       <c r="N37" s="14">
-        <v>50000</v>
+        <v>12500</v>
       </c>
       <c r="O37" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -2986,19 +3076,19 @@
         <v>45945</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="F38" s="12">
-        <v>773199049</v>
+        <v>786323232</v>
       </c>
       <c r="G38" s="12" t="s">
         <v>16</v>
@@ -3010,19 +3100,19 @@
         <v>17</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="L38" s="12">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="M38" s="14">
-        <v>10250</v>
+        <v>26000</v>
       </c>
       <c r="N38" s="14">
-        <v>51250</v>
+        <v>650000</v>
       </c>
       <c r="O38" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -3038,19 +3128,19 @@
         <v>45945</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="F39" s="12">
-        <v>779676016</v>
+        <v>784537895</v>
       </c>
       <c r="G39" s="12" t="s">
         <v>16</v>
@@ -3062,19 +3152,19 @@
         <v>17</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L39" s="12">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="M39" s="14">
-        <v>12500</v>
+        <v>15500</v>
       </c>
       <c r="N39" s="14">
-        <v>312500</v>
+        <v>15500</v>
       </c>
       <c r="O39" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -3090,19 +3180,19 @@
         <v>45945</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="F40" s="12">
-        <v>773199049</v>
+        <v>784537895</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>16</v>
@@ -3114,19 +3204,19 @@
         <v>17</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="L40" s="12">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="M40" s="14">
-        <v>6000</v>
+        <v>12500</v>
       </c>
       <c r="N40" s="14">
-        <v>150000</v>
+        <v>12500</v>
       </c>
       <c r="O40" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -3142,22 +3232,22 @@
         <v>45945</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="F41" s="12">
-        <v>773482683</v>
+        <v>775541532</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="H41" s="12" t="s">
         <v>13</v>
@@ -3166,12 +3256,20 @@
         <v>17</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="K41" s="12"/>
-      <c r="L41" s="12"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="K41" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L41" s="12">
+        <v>10</v>
+      </c>
+      <c r="M41" s="14">
+        <v>9750</v>
+      </c>
+      <c r="N41" s="14">
+        <v>97500</v>
+      </c>
       <c r="O41" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S42</v>
@@ -3186,19 +3284,19 @@
         <v>45945</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F42" s="12">
-        <v>770712599</v>
+        <v>774540865</v>
       </c>
       <c r="G42" s="12" t="s">
         <v>16</v>
@@ -3210,19 +3308,19 @@
         <v>17</v>
       </c>
       <c r="J42" s="13" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="L42" s="12">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="M42" s="14">
-        <v>26000</v>
+        <v>15500</v>
       </c>
       <c r="N42" s="14">
-        <v>1300000</v>
+        <v>15500</v>
       </c>
       <c r="O42" s="9" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
@@ -3233,24 +3331,24 @@
         <v>octobre</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="28.15" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A43" s="11">
         <v>45945</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F43" s="12">
-        <v>774024173</v>
+        <v>775405469</v>
       </c>
       <c r="G43" s="12" t="s">
         <v>16</v>
@@ -3262,25 +3360,857 @@
         <v>17</v>
       </c>
       <c r="J43" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K43" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L43" s="12">
+        <v>5</v>
+      </c>
+      <c r="M43" s="14">
+        <v>19500</v>
+      </c>
+      <c r="N43" s="14">
+        <v>97500</v>
+      </c>
+      <c r="O43" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P43" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A44" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="12">
+        <v>774245132</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I44" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J44" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L44" s="12">
+        <v>5</v>
+      </c>
+      <c r="M44" s="14">
+        <v>19500</v>
+      </c>
+      <c r="N44" s="14">
+        <v>97500</v>
+      </c>
+      <c r="O44" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P44" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A45" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F45" s="12">
+        <v>771428937</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K45" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L45" s="12">
+        <v>25</v>
+      </c>
+      <c r="M45" s="14">
+        <v>26000</v>
+      </c>
+      <c r="N45" s="14">
+        <v>650000</v>
+      </c>
+      <c r="O45" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P45" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A46" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F46" s="12">
+        <v>785554540</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K46" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L46" s="12">
+        <v>1</v>
+      </c>
+      <c r="M46" s="14">
+        <v>15500</v>
+      </c>
+      <c r="N46" s="14">
+        <v>15500</v>
+      </c>
+      <c r="O46" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P46" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A47" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F47" s="12">
+        <v>773756258</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J47" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K47" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L47" s="12">
+        <v>5</v>
+      </c>
+      <c r="M47" s="14">
+        <v>19500</v>
+      </c>
+      <c r="N47" s="14">
+        <v>97500</v>
+      </c>
+      <c r="O47" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P47" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A48" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F48" s="12">
+        <v>773777037</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I48" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J48" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K48" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L48" s="12">
+        <v>25</v>
+      </c>
+      <c r="M48" s="14">
+        <v>26000</v>
+      </c>
+      <c r="N48" s="14">
+        <v>650000</v>
+      </c>
+      <c r="O48" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P48" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A49" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F49" s="12">
+        <v>773750007</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I49" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J49" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K49" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L49" s="12">
+        <v>2</v>
+      </c>
+      <c r="M49" s="14">
+        <v>15500</v>
+      </c>
+      <c r="N49" s="14">
+        <v>31000</v>
+      </c>
+      <c r="O49" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P49" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A50" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F50" s="12">
+        <v>773750007</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J50" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K50" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L50" s="12">
+        <v>1</v>
+      </c>
+      <c r="M50" s="14">
+        <v>15500</v>
+      </c>
+      <c r="N50" s="14">
+        <v>15500</v>
+      </c>
+      <c r="O50" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P50" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A51" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F51" s="12">
+        <v>775171537</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H51" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I51" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K51" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L51" s="12">
+        <v>25</v>
+      </c>
+      <c r="M51" s="14">
+        <v>26000</v>
+      </c>
+      <c r="N51" s="14">
+        <v>650000</v>
+      </c>
+      <c r="O51" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P51" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A52" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F52" s="12">
+        <v>779676016</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H52" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J52" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K52" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="L52" s="12">
+        <v>25</v>
+      </c>
+      <c r="M52" s="14">
+        <v>12500</v>
+      </c>
+      <c r="N52" s="14">
+        <v>312500</v>
+      </c>
+      <c r="O52" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P52" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A53" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F53" s="12">
+        <v>773199049</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I53" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J53" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K53" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L53" s="12">
+        <v>25</v>
+      </c>
+      <c r="M53" s="14">
+        <v>6000</v>
+      </c>
+      <c r="N53" s="14">
+        <v>150000</v>
+      </c>
+      <c r="O53" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P53" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A54" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F54" s="12">
+        <v>773199049</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H54" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I54" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J54" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K54" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="L54" s="12">
+        <v>5</v>
+      </c>
+      <c r="M54" s="14">
+        <v>10000</v>
+      </c>
+      <c r="N54" s="14">
+        <v>50000</v>
+      </c>
+      <c r="O54" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P54" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A55" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F55" s="12">
+        <v>773199049</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I55" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J55" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K55" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L55" s="12">
+        <v>5</v>
+      </c>
+      <c r="M55" s="14">
+        <v>10250</v>
+      </c>
+      <c r="N55" s="14">
+        <v>51250</v>
+      </c>
+      <c r="O55" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P55" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A56" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F56" s="12">
+        <v>776818022</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H56" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J56" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K56" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L56" s="12">
+        <v>25</v>
+      </c>
+      <c r="M56" s="14">
+        <v>9750</v>
+      </c>
+      <c r="N56" s="14">
+        <v>243750</v>
+      </c>
+      <c r="O56" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P56" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A57" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F57" s="12">
+        <v>773482683</v>
+      </c>
+      <c r="G57" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H57" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I57" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J57" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="K57" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="L57" s="12">
+        <v>25</v>
+      </c>
+      <c r="M57" s="14">
+        <v>31000</v>
+      </c>
+      <c r="N57" s="14">
+        <v>775000</v>
+      </c>
+      <c r="O57" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P57" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="28.15" x14ac:dyDescent="0.45">
+      <c r="A58" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F58" s="12">
+        <v>774024173</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H58" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J58" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="K43" s="12" t="s">
+      <c r="K58" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="L43" s="12">
+      <c r="L58" s="12">
         <v>50</v>
       </c>
-      <c r="M43" s="14">
+      <c r="M58" s="14">
         <v>26000</v>
       </c>
-      <c r="N43" s="14">
+      <c r="N58" s="14">
         <v>1300000</v>
       </c>
-      <c r="O43" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P43" s="10" t="str">
+      <c r="O58" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P58" s="10" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A59" s="11">
+        <v>45945</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F59" s="12">
+        <v>770712599</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H59" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J59" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="K59" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L59" s="12">
+        <v>50</v>
+      </c>
+      <c r="M59" s="14">
+        <v>26000</v>
+      </c>
+      <c r="N59" s="14">
+        <v>1300000</v>
+      </c>
+      <c r="O59" s="9" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P59" s="10" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>

</xml_diff>

<commit_message>
Rapport du 22 Octobre 2025
</commit_message>
<xml_diff>
--- a/Donnees_RZ.xlsx
+++ b/Donnees_RZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D918D3-00AA-41A0-90AD-BFCFD3A0E13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01447637-E130-4293-837A-45A549603C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="136">
   <si>
     <t>Date</t>
   </si>
@@ -420,6 +420,28 @@
   </si>
   <si>
     <t>Café Altimo pot 200g x 12 pcs</t>
+  </si>
+  <si>
+    <t>Ouakam</t>
+  </si>
+  <si>
+    <t>Ibrahima Sori Diallo</t>
+  </si>
+  <si>
+    <t>Commande reçue très tardivement.il avait déjà fermé il a trop attendu</t>
+  </si>
+  <si>
+    <t>Bassoum khamza</t>
+  </si>
+  <si>
+    <t>Abdoulaye  Ba 
+A</t>
+  </si>
+  <si>
+    <t>Moustapha  seye</t>
+  </si>
+  <si>
+    <t>Améne le reste demain stp</t>
   </si>
 </sst>
 </file>
@@ -487,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -509,21 +531,46 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -564,40 +611,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-        <name val="TIMES"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -624,6 +637,7 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -750,6 +764,20 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color auto="1"/>
@@ -810,27 +838,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P59" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A1:P59" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P67" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A1:P67" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{F85C405C-E78B-4DA6-8568-08107D7551E4}" name="Date" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{24A95AD6-D6B8-4864-9451-50BFB3565C62}" name="Prenom_Nom_RZ" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{72E50CE0-52B1-4C49-9D23-C97154D649A5}" name="zone" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{E26577ED-9647-48EE-BE53-9D2F344CB36B}" name="secteur" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{43164A48-AFB0-417D-94C4-5347A67ACD14}" name="Nom_du_magasin" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{66D926A0-8C65-4D89-BA92-AA9653C7DE06}" name="Telephone_Client" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{8D4D921E-310A-44FC-AA1D-F30B627C5984}" name="Type" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{636AF8A9-C9D0-49B6-94C8-FFB87B44FA47}" name="Point_de_Vente" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{35E41B20-D7EB-4025-A9CC-62B85956ABCD}" name="Operation" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{AB905DE1-CC5E-4C11-8318-9C04B6D96EC3}" name="Commentaire" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{9BC88C3B-EEBD-4156-81CB-075746F3F057}" name="Produit" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{8DD706C4-BCF7-47C0-9913-F482F7A2F321}" name="Quantites" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{D96EE09E-B22B-4D75-AABE-AEBF7CE286A6}" name="Prix_Unitaire" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{B1727D51-96B6-4015-83C5-EBCAD96E9834}" name="Prix Total" dataDxfId="0"/>
-    <tableColumn id="17" xr3:uid="{9A2C6D78-CE06-4E13-B8E1-0CB92B201156}" name="Semaine" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{F85C405C-E78B-4DA6-8568-08107D7551E4}" name="Date" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{24A95AD6-D6B8-4864-9451-50BFB3565C62}" name="Prenom_Nom_RZ" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{72E50CE0-52B1-4C49-9D23-C97154D649A5}" name="zone" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{E26577ED-9647-48EE-BE53-9D2F344CB36B}" name="secteur" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{43164A48-AFB0-417D-94C4-5347A67ACD14}" name="Nom_du_magasin" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{66D926A0-8C65-4D89-BA92-AA9653C7DE06}" name="Telephone_Client" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{8D4D921E-310A-44FC-AA1D-F30B627C5984}" name="Type" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{636AF8A9-C9D0-49B6-94C8-FFB87B44FA47}" name="Point_de_Vente" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{35E41B20-D7EB-4025-A9CC-62B85956ABCD}" name="Operation" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{AB905DE1-CC5E-4C11-8318-9C04B6D96EC3}" name="Commentaire" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{9BC88C3B-EEBD-4156-81CB-075746F3F057}" name="Produit" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{8DD706C4-BCF7-47C0-9913-F482F7A2F321}" name="Quantites" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{D96EE09E-B22B-4D75-AABE-AEBF7CE286A6}" name="Prix_Unitaire" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{B1727D51-96B6-4015-83C5-EBCAD96E9834}" name="Prix Total" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{9A2C6D78-CE06-4E13-B8E1-0CB92B201156}" name="Semaine" dataDxfId="1">
       <calculatedColumnFormula>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{83F3E9A5-7911-47C6-B543-07173CE7D4B5}" name="Mois" dataDxfId="4">
+    <tableColumn id="18" xr3:uid="{83F3E9A5-7911-47C6-B543-07173CE7D4B5}" name="Mois" dataDxfId="0">
       <calculatedColumnFormula>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1124,10 +1152,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:P59"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D39" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView tabSelected="1" topLeftCell="I39" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="T64" sqref="T64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1242,11 +1270,11 @@
       <c r="N2" s="4">
         <v>387500</v>
       </c>
-      <c r="O2" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P2" s="10" t="str">
+      <c r="O2" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P2" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
@@ -1294,2923 +1322,3339 @@
       <c r="N3" s="4">
         <v>312500</v>
       </c>
-      <c r="O3" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P3" s="10" t="str">
+      <c r="O3" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P3" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A4" s="11">
+      <c r="A4" s="9">
         <v>45947</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="10">
         <v>771701320</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="13" t="s">
+      <c r="H4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="10">
         <v>25</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="12">
         <v>9750</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="12">
         <v>243750</v>
       </c>
-      <c r="O4" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P4" s="10" t="str">
+      <c r="O4" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P4" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A5" s="11">
+      <c r="A5" s="9">
         <v>45947</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="10">
         <v>772494182</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="13" t="s">
+      <c r="I5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="10">
         <v>5</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="12">
         <v>9750</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="12">
         <v>48750</v>
       </c>
-      <c r="O5" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P5" s="10" t="str">
+      <c r="O5" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P5" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A6" s="11">
+      <c r="A6" s="9">
         <v>45947</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="10">
         <v>764881522</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="13" t="s">
+      <c r="H6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="10">
         <v>5</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="12">
         <v>19500</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="12">
         <v>97500</v>
       </c>
-      <c r="O6" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P6" s="10" t="str">
+      <c r="O6" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P6" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A7" s="11">
+      <c r="A7" s="9">
         <v>45947</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="10">
         <v>772884203</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="13" t="s">
+      <c r="H7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="10">
         <v>5</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M7" s="12">
         <v>19500</v>
       </c>
-      <c r="N7" s="14">
+      <c r="N7" s="12">
         <v>97500</v>
       </c>
-      <c r="O7" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P7" s="10" t="str">
+      <c r="O7" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P7" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A8" s="11">
+      <c r="A8" s="9">
         <v>45946</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="10">
         <v>771987678</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="13" t="s">
+      <c r="I8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="10">
         <v>25</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="12">
         <v>11500</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="12">
         <v>287500</v>
       </c>
-      <c r="O8" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P8" s="10" t="str">
+      <c r="O8" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P8" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A9" s="11">
+      <c r="A9" s="9">
         <v>45947</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="10">
         <v>775538380</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="13" t="s">
+      <c r="I9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="10">
         <v>1</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9" s="12">
         <v>19500</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9" s="12">
         <v>19500</v>
       </c>
-      <c r="O9" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P9" s="10" t="str">
+      <c r="O9" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P9" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A10" s="11">
+      <c r="A10" s="9">
         <v>45947</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="10">
         <v>775987400</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="13" t="s">
+      <c r="I10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="10">
         <v>1</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="12">
         <v>19500</v>
       </c>
-      <c r="N10" s="14">
+      <c r="N10" s="12">
         <v>19500</v>
       </c>
-      <c r="O10" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P10" s="10" t="str">
+      <c r="O10" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P10" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A11" s="11">
+      <c r="A11" s="9">
         <v>45947</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="10">
         <v>773170826</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="13" t="s">
+      <c r="H11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="10">
         <v>2</v>
       </c>
-      <c r="M11" s="14">
+      <c r="M11" s="12">
         <v>19500</v>
       </c>
-      <c r="N11" s="14">
+      <c r="N11" s="12">
         <v>39000</v>
       </c>
-      <c r="O11" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P11" s="10" t="str">
+      <c r="O11" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P11" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A12" s="11">
+      <c r="A12" s="9">
         <v>45947</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="10">
         <v>777972938</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" s="13" t="s">
+      <c r="I12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="10">
         <v>1</v>
       </c>
-      <c r="M12" s="14">
+      <c r="M12" s="12">
         <v>12500</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N12" s="12">
         <v>12500</v>
       </c>
-      <c r="O12" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P12" s="10" t="str">
+      <c r="O12" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P12" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A13" s="11">
+      <c r="A13" s="9">
         <v>45947</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="10">
         <v>772900705</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="13" t="s">
+      <c r="I13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="K13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="10">
         <v>1</v>
       </c>
-      <c r="M13" s="14">
+      <c r="M13" s="12">
         <v>26000</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="12">
         <v>26000</v>
       </c>
-      <c r="O13" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P13" s="10" t="str">
+      <c r="O13" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P13" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A14" s="11">
+      <c r="A14" s="9">
         <v>45947</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="10">
         <v>776167544</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="13" t="s">
+      <c r="H14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="K14" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="10">
         <v>2</v>
       </c>
-      <c r="M14" s="14">
+      <c r="M14" s="12">
         <v>11500</v>
       </c>
-      <c r="N14" s="14">
+      <c r="N14" s="12">
         <v>23000</v>
       </c>
-      <c r="O14" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P14" s="10" t="str">
+      <c r="O14" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P14" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A15" s="11">
+      <c r="A15" s="9">
         <v>45947</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="10">
         <v>775884054</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="13" t="s">
+      <c r="H15" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="L15" s="12">
+      <c r="L15" s="10">
         <v>1</v>
       </c>
-      <c r="M15" s="14">
+      <c r="M15" s="12">
         <v>31000</v>
       </c>
-      <c r="N15" s="14">
+      <c r="N15" s="12">
         <v>31000</v>
       </c>
-      <c r="O15" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P15" s="10" t="str">
+      <c r="O15" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P15" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A16" s="11">
+      <c r="A16" s="9">
         <v>45947</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="10">
         <v>772131614</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J16" s="13" t="s">
+      <c r="H16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="10">
         <v>1</v>
       </c>
-      <c r="M16" s="14">
+      <c r="M16" s="12">
         <v>26000</v>
       </c>
-      <c r="N16" s="14">
+      <c r="N16" s="12">
         <v>26000</v>
       </c>
-      <c r="O16" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P16" s="10" t="str">
+      <c r="O16" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P16" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A17" s="11">
+      <c r="A17" s="9">
         <v>45947</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="10">
         <v>774446616</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="H17" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J17" s="13" t="s">
+      <c r="H17" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="L17" s="12">
+      <c r="L17" s="10">
         <v>1</v>
       </c>
-      <c r="M17" s="14">
+      <c r="M17" s="12">
         <v>15500</v>
       </c>
-      <c r="N17" s="14">
+      <c r="N17" s="12">
         <v>15500</v>
       </c>
-      <c r="O17" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P17" s="10" t="str">
+      <c r="O17" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P17" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A18" s="11">
+      <c r="A18" s="9">
         <v>45946</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="10">
         <v>776212473</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="13" t="s">
+      <c r="H18" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="K18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L18" s="12">
-        <v>13</v>
-      </c>
-      <c r="M18" s="14">
+      <c r="L18" s="10">
+        <v>13</v>
+      </c>
+      <c r="M18" s="12">
         <v>19500</v>
       </c>
-      <c r="N18" s="14">
+      <c r="N18" s="12">
         <v>253500</v>
       </c>
-      <c r="O18" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P18" s="10" t="str">
+      <c r="O18" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P18" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A19" s="11">
+      <c r="A19" s="9">
         <v>45946</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="10">
         <v>784426640</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" s="13" t="s">
+      <c r="H19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="K19" s="12" t="s">
+      <c r="K19" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="10">
         <v>25</v>
       </c>
-      <c r="M19" s="14">
+      <c r="M19" s="12">
         <v>11500</v>
       </c>
-      <c r="N19" s="14">
+      <c r="N19" s="12">
         <v>287500</v>
       </c>
-      <c r="O19" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P19" s="10" t="str">
+      <c r="O19" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P19" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A20" s="11">
+      <c r="A20" s="9">
         <v>45945</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="10">
         <v>771010134</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" s="13" t="s">
+      <c r="H20" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="K20" s="12" t="s">
+      <c r="K20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="12">
+      <c r="L20" s="10">
         <v>100</v>
       </c>
-      <c r="M20" s="14">
+      <c r="M20" s="12">
         <v>26000</v>
       </c>
-      <c r="N20" s="14">
+      <c r="N20" s="12">
         <v>2600000</v>
       </c>
-      <c r="O20" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P20" s="10" t="str">
+      <c r="O20" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P20" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A21" s="11">
+      <c r="A21" s="9">
         <v>45946</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="10">
         <v>773340367</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J21" s="13" t="s">
+      <c r="H21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K21" s="12" t="s">
+      <c r="K21" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L21" s="10">
         <v>12</v>
       </c>
-      <c r="M21" s="14">
+      <c r="M21" s="12">
         <v>19500</v>
       </c>
-      <c r="N21" s="14">
+      <c r="N21" s="12">
         <v>234000</v>
       </c>
-      <c r="O21" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P21" s="10" t="str">
+      <c r="O21" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P21" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A22" s="11">
+      <c r="A22" s="9">
         <v>45946</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="10">
         <v>775894235</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J22" s="13" t="s">
+      <c r="H22" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="K22" s="12" t="s">
+      <c r="K22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="10">
         <v>1</v>
       </c>
-      <c r="M22" s="14">
+      <c r="M22" s="12">
         <v>19500</v>
       </c>
-      <c r="N22" s="14">
+      <c r="N22" s="12">
         <v>19500</v>
       </c>
-      <c r="O22" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P22" s="10" t="str">
+      <c r="O22" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P22" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A23" s="11">
+      <c r="A23" s="9">
         <v>45946</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="10">
         <v>775894235</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="13" t="s">
+      <c r="H23" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="K23" s="12" t="s">
+      <c r="K23" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="L23" s="12">
+      <c r="L23" s="10">
         <v>5</v>
       </c>
-      <c r="M23" s="14">
+      <c r="M23" s="12">
         <v>33500</v>
       </c>
-      <c r="N23" s="14">
+      <c r="N23" s="12">
         <v>167500</v>
       </c>
-      <c r="O23" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P23" s="10" t="str">
+      <c r="O23" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P23" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A24" s="11">
+      <c r="A24" s="9">
         <v>45946</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="10">
         <v>775894235</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="G24" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H24" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I24" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24" s="13" t="s">
+      <c r="H24" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="K24" s="12" t="s">
+      <c r="K24" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="L24" s="12">
+      <c r="L24" s="10">
         <v>4</v>
       </c>
-      <c r="M24" s="14">
+      <c r="M24" s="12">
         <v>34500</v>
       </c>
-      <c r="N24" s="14">
+      <c r="N24" s="12">
         <v>138000</v>
       </c>
-      <c r="O24" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P24" s="10" t="str">
+      <c r="O24" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P24" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A25" s="11">
+      <c r="A25" s="9">
         <v>45945</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25" s="10">
         <v>773199049</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G25" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J25" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K25" s="12" t="s">
+      <c r="H25" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K25" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="L25" s="12">
+      <c r="L25" s="10">
         <v>25</v>
       </c>
-      <c r="M25" s="14">
+      <c r="M25" s="12">
         <v>6000</v>
       </c>
-      <c r="N25" s="14">
+      <c r="N25" s="12">
         <v>150000</v>
       </c>
-      <c r="O25" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P25" s="10" t="str">
+      <c r="O25" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P25" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A26" s="11">
+      <c r="A26" s="9">
         <v>45945</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="10">
         <v>775273147</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="G26" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I26" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J26" s="13" t="s">
+      <c r="H26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="K26" s="12" t="s">
+      <c r="K26" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="L26" s="12">
+      <c r="L26" s="10">
         <v>1</v>
       </c>
-      <c r="M26" s="14">
+      <c r="M26" s="12">
         <v>12500</v>
       </c>
-      <c r="N26" s="14">
+      <c r="N26" s="12">
         <v>12500</v>
       </c>
-      <c r="O26" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P26" s="10" t="str">
+      <c r="O26" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P26" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A27" s="11">
+      <c r="A27" s="9">
         <v>45945</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="10">
         <v>775273147</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J27" s="13" t="s">
+      <c r="H27" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="K27" s="12" t="s">
+      <c r="K27" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="L27" s="12">
+      <c r="L27" s="10">
         <v>25</v>
       </c>
-      <c r="M27" s="14">
+      <c r="M27" s="12">
         <v>6000</v>
       </c>
-      <c r="N27" s="14">
+      <c r="N27" s="12">
         <v>150000</v>
       </c>
-      <c r="O27" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P27" s="10" t="str">
+      <c r="O27" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P27" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A28" s="11">
+      <c r="A28" s="9">
         <v>45945</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="10">
         <v>775273147</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H28" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J28" s="13" t="s">
+      <c r="H28" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="K28" s="12" t="s">
+      <c r="K28" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L28" s="12">
+      <c r="L28" s="10">
         <v>2</v>
       </c>
-      <c r="M28" s="14">
+      <c r="M28" s="12">
         <v>26000</v>
       </c>
-      <c r="N28" s="14">
+      <c r="N28" s="12">
         <v>52000</v>
       </c>
-      <c r="O28" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P28" s="10" t="str">
+      <c r="O28" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P28" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A29" s="11">
+      <c r="A29" s="9">
         <v>45945</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E29" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29" s="10">
         <v>775273147</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="G29" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J29" s="13" t="s">
+      <c r="H29" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="K29" s="12" t="s">
+      <c r="K29" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="L29" s="12">
+      <c r="L29" s="10">
         <v>1</v>
       </c>
-      <c r="M29" s="14">
+      <c r="M29" s="12">
         <v>10000</v>
       </c>
-      <c r="N29" s="14">
+      <c r="N29" s="12">
         <v>10000</v>
       </c>
-      <c r="O29" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P29" s="10" t="str">
+      <c r="O29" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P29" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A30" s="11">
+      <c r="A30" s="9">
         <v>45945</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30" s="10">
         <v>767379110</v>
       </c>
-      <c r="G30" s="12" t="s">
+      <c r="G30" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J30" s="13" t="s">
+      <c r="H30" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K30" s="12" t="s">
+      <c r="K30" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="L30" s="12">
+      <c r="L30" s="10">
         <v>7</v>
       </c>
-      <c r="M30" s="14">
+      <c r="M30" s="12">
         <v>15500</v>
       </c>
-      <c r="N30" s="14">
+      <c r="N30" s="12">
         <v>108500</v>
       </c>
-      <c r="O30" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P30" s="10" t="str">
+      <c r="O30" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P30" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A31" s="11">
+      <c r="A31" s="9">
         <v>45945</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="10">
         <v>763469670</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="G31" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H31" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I31" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J31" s="13" t="s">
+      <c r="H31" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K31" s="12" t="s">
+      <c r="K31" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L31" s="12">
+      <c r="L31" s="10">
         <v>100</v>
       </c>
-      <c r="M31" s="14">
+      <c r="M31" s="12">
         <v>26000</v>
       </c>
-      <c r="N31" s="14">
+      <c r="N31" s="12">
         <v>2600000</v>
       </c>
-      <c r="O31" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P31" s="10" t="str">
+      <c r="O31" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P31" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A32" s="11">
+      <c r="A32" s="9">
         <v>45945</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F32" s="12">
+      <c r="F32" s="10">
         <v>781757464</v>
       </c>
-      <c r="G32" s="12" t="s">
+      <c r="G32" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H32" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J32" s="13" t="s">
+      <c r="H32" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K32" s="12" t="s">
+      <c r="K32" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L32" s="12">
+      <c r="L32" s="10">
         <v>5</v>
       </c>
-      <c r="M32" s="14">
+      <c r="M32" s="12">
         <v>19500</v>
       </c>
-      <c r="N32" s="14">
+      <c r="N32" s="12">
         <v>97500</v>
       </c>
-      <c r="O32" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P32" s="10" t="str">
+      <c r="O32" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P32" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A33" s="11">
+      <c r="A33" s="9">
         <v>45945</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F33" s="12">
+      <c r="F33" s="10">
         <v>774540865</v>
       </c>
-      <c r="G33" s="12" t="s">
+      <c r="G33" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I33" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J33" s="13" t="s">
+      <c r="H33" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K33" s="12" t="s">
+      <c r="K33" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="L33" s="12">
+      <c r="L33" s="10">
         <v>1</v>
       </c>
-      <c r="M33" s="14">
+      <c r="M33" s="12">
         <v>12500</v>
       </c>
-      <c r="N33" s="14">
+      <c r="N33" s="12">
         <v>12500</v>
       </c>
-      <c r="O33" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P33" s="10" t="str">
+      <c r="O33" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P33" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A34" s="11">
+      <c r="A34" s="9">
         <v>45945</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34" s="10">
         <v>771010134</v>
       </c>
-      <c r="G34" s="12" t="s">
+      <c r="G34" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H34" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I34" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J34" s="13" t="s">
+      <c r="H34" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J34" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="K34" s="12" t="s">
+      <c r="K34" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="L34" s="12">
+      <c r="L34" s="10">
         <v>1</v>
       </c>
-      <c r="M34" s="14">
+      <c r="M34" s="12">
         <v>10000</v>
       </c>
-      <c r="N34" s="14">
+      <c r="N34" s="12">
         <v>10000</v>
       </c>
-      <c r="O34" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P34" s="10" t="str">
+      <c r="O34" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P34" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A35" s="11">
+      <c r="A35" s="9">
         <v>45945</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F35" s="12">
+      <c r="F35" s="10">
         <v>771010134</v>
       </c>
-      <c r="G35" s="12" t="s">
+      <c r="G35" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H35" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I35" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J35" s="13" t="s">
+      <c r="H35" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="K35" s="12" t="s">
+      <c r="K35" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="L35" s="12">
+      <c r="L35" s="10">
         <v>1</v>
       </c>
-      <c r="M35" s="14">
+      <c r="M35" s="12">
         <v>15500</v>
       </c>
-      <c r="N35" s="14">
+      <c r="N35" s="12">
         <v>15500</v>
       </c>
-      <c r="O35" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P35" s="10" t="str">
+      <c r="O35" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P35" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A36" s="11">
+      <c r="A36" s="9">
         <v>45945</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F36" s="12">
+      <c r="F36" s="10">
         <v>771010134</v>
       </c>
-      <c r="G36" s="12" t="s">
+      <c r="G36" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H36" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I36" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J36" s="13" t="s">
+      <c r="H36" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="K36" s="12" t="s">
+      <c r="K36" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="L36" s="12">
+      <c r="L36" s="10">
         <v>1</v>
       </c>
-      <c r="M36" s="14">
+      <c r="M36" s="12">
         <v>12500</v>
       </c>
-      <c r="N36" s="14">
+      <c r="N36" s="12">
         <v>12500</v>
       </c>
-      <c r="O36" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P36" s="10" t="str">
+      <c r="O36" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P36" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A37" s="11">
+      <c r="A37" s="9">
         <v>45943</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F37" s="12">
+      <c r="F37" s="10">
         <v>775772788</v>
       </c>
-      <c r="G37" s="12" t="s">
+      <c r="G37" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H37" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I37" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J37" s="13" t="s">
+      <c r="H37" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K37" s="12" t="s">
+      <c r="K37" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L37" s="12">
+      <c r="L37" s="10">
         <v>50</v>
       </c>
-      <c r="M37" s="14">
+      <c r="M37" s="12">
         <v>26000</v>
       </c>
-      <c r="N37" s="14">
+      <c r="N37" s="12">
         <v>1300000</v>
       </c>
-      <c r="O37" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P37" s="10" t="str">
+      <c r="O37" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P37" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A38" s="11">
+      <c r="A38" s="9">
         <v>45945</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F38" s="12">
+      <c r="F38" s="10">
         <v>786323232</v>
       </c>
-      <c r="G38" s="12" t="s">
+      <c r="G38" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H38" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I38" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J38" s="13" t="s">
+      <c r="H38" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K38" s="12" t="s">
+      <c r="K38" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L38" s="12">
+      <c r="L38" s="10">
         <v>25</v>
       </c>
-      <c r="M38" s="14">
+      <c r="M38" s="12">
         <v>19500</v>
       </c>
-      <c r="N38" s="14">
+      <c r="N38" s="12">
         <v>487500</v>
       </c>
-      <c r="O38" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P38" s="10" t="str">
+      <c r="O38" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P38" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A39" s="11">
+      <c r="A39" s="9">
         <v>45945</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F39" s="12">
+      <c r="F39" s="10">
         <v>784537895</v>
       </c>
-      <c r="G39" s="12" t="s">
+      <c r="G39" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H39" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I39" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="13" t="s">
+      <c r="H39" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I39" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K39" s="12" t="s">
+      <c r="K39" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="L39" s="12">
+      <c r="L39" s="10">
         <v>1</v>
       </c>
-      <c r="M39" s="14">
+      <c r="M39" s="12">
         <v>15500</v>
       </c>
-      <c r="N39" s="14">
+      <c r="N39" s="12">
         <v>15500</v>
       </c>
-      <c r="O39" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P39" s="10" t="str">
+      <c r="O39" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P39" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A40" s="11">
+      <c r="A40" s="9">
         <v>45945</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="12">
+      <c r="F40" s="10">
         <v>784537895</v>
       </c>
-      <c r="G40" s="12" t="s">
+      <c r="G40" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H40" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I40" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J40" s="13" t="s">
+      <c r="H40" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K40" s="12" t="s">
+      <c r="K40" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="L40" s="12">
+      <c r="L40" s="10">
         <v>1</v>
       </c>
-      <c r="M40" s="14">
+      <c r="M40" s="12">
         <v>12500</v>
       </c>
-      <c r="N40" s="14">
+      <c r="N40" s="12">
         <v>12500</v>
       </c>
-      <c r="O40" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P40" s="10" t="str">
+      <c r="O40" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P40" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A41" s="11">
+      <c r="A41" s="9">
         <v>45945</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F41" s="12">
+      <c r="F41" s="10">
         <v>775541532</v>
       </c>
-      <c r="G41" s="12" t="s">
+      <c r="G41" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H41" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I41" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J41" s="13" t="s">
+      <c r="H41" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K41" s="12" t="s">
+      <c r="K41" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="L41" s="12">
+      <c r="L41" s="10">
         <v>10</v>
       </c>
-      <c r="M41" s="14">
+      <c r="M41" s="12">
         <v>9750</v>
       </c>
-      <c r="N41" s="14">
+      <c r="N41" s="12">
         <v>102500</v>
       </c>
-      <c r="O41" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P41" s="10" t="str">
+      <c r="O41" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P41" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A42" s="11">
+      <c r="A42" s="9">
         <v>45945</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F42" s="12">
+      <c r="F42" s="10">
         <v>774540865</v>
       </c>
-      <c r="G42" s="12" t="s">
+      <c r="G42" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H42" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I42" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J42" s="13" t="s">
+      <c r="H42" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K42" s="12" t="s">
+      <c r="K42" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="L42" s="12">
+      <c r="L42" s="10">
         <v>1</v>
       </c>
-      <c r="M42" s="14">
+      <c r="M42" s="12">
         <v>15500</v>
       </c>
-      <c r="N42" s="14">
+      <c r="N42" s="12">
         <v>15500</v>
       </c>
-      <c r="O42" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P42" s="10" t="str">
+      <c r="O42" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P42" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A43" s="11">
+      <c r="A43" s="9">
         <v>45945</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F43" s="12">
+      <c r="F43" s="10">
         <v>775405469</v>
       </c>
-      <c r="G43" s="12" t="s">
+      <c r="G43" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H43" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I43" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J43" s="13" t="s">
+      <c r="H43" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J43" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K43" s="12" t="s">
+      <c r="K43" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L43" s="12">
+      <c r="L43" s="10">
         <v>5</v>
       </c>
-      <c r="M43" s="14">
+      <c r="M43" s="12">
         <v>19500</v>
       </c>
-      <c r="N43" s="14">
+      <c r="N43" s="12">
         <v>97500</v>
       </c>
-      <c r="O43" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P43" s="10" t="str">
+      <c r="O43" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P43" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A44" s="11">
+      <c r="A44" s="9">
         <v>45945</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F44" s="12">
+      <c r="F44" s="10">
         <v>774245132</v>
       </c>
-      <c r="G44" s="12" t="s">
+      <c r="G44" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H44" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I44" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J44" s="13" t="s">
+      <c r="H44" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J44" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K44" s="12" t="s">
+      <c r="K44" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L44" s="12">
+      <c r="L44" s="10">
         <v>5</v>
       </c>
-      <c r="M44" s="14">
+      <c r="M44" s="12">
         <v>19500</v>
       </c>
-      <c r="N44" s="14">
+      <c r="N44" s="12">
         <v>97500</v>
       </c>
-      <c r="O44" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P44" s="10" t="str">
+      <c r="O44" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P44" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A45" s="11">
+      <c r="A45" s="9">
         <v>45945</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C45" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="E45" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F45" s="12">
+      <c r="F45" s="10">
         <v>771428937</v>
       </c>
-      <c r="G45" s="12" t="s">
+      <c r="G45" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H45" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I45" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J45" s="13" t="s">
+      <c r="H45" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K45" s="12" t="s">
+      <c r="K45" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L45" s="12">
+      <c r="L45" s="10">
         <v>25</v>
       </c>
-      <c r="M45" s="14">
+      <c r="M45" s="12">
         <v>26000</v>
       </c>
-      <c r="N45" s="14">
+      <c r="N45" s="12">
         <v>650000</v>
       </c>
-      <c r="O45" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P45" s="10" t="str">
+      <c r="O45" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P45" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A46" s="11">
+      <c r="A46" s="9">
         <v>45945</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F46" s="12">
+      <c r="F46" s="10">
         <v>785554540</v>
       </c>
-      <c r="G46" s="12" t="s">
+      <c r="G46" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H46" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I46" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J46" s="13" t="s">
+      <c r="H46" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K46" s="12" t="s">
+      <c r="K46" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="L46" s="12">
+      <c r="L46" s="10">
         <v>1</v>
       </c>
-      <c r="M46" s="14">
+      <c r="M46" s="12">
         <v>15500</v>
       </c>
-      <c r="N46" s="14">
+      <c r="N46" s="12">
         <v>15500</v>
       </c>
-      <c r="O46" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P46" s="10" t="str">
+      <c r="O46" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P46" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A47" s="11">
+      <c r="A47" s="9">
         <v>45945</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="E47" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F47" s="12">
+      <c r="F47" s="10">
         <v>773756258</v>
       </c>
-      <c r="G47" s="12" t="s">
+      <c r="G47" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I47" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J47" s="13" t="s">
+      <c r="H47" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J47" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K47" s="12" t="s">
+      <c r="K47" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L47" s="12">
+      <c r="L47" s="10">
         <v>5</v>
       </c>
-      <c r="M47" s="14">
+      <c r="M47" s="12">
         <v>19500</v>
       </c>
-      <c r="N47" s="14">
+      <c r="N47" s="12">
         <v>97500</v>
       </c>
-      <c r="O47" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P47" s="10" t="str">
+      <c r="O47" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P47" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A48" s="11">
+      <c r="A48" s="9">
         <v>45945</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B48" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C48" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E48" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F48" s="12">
+      <c r="F48" s="10">
         <v>773777037</v>
       </c>
-      <c r="G48" s="12" t="s">
+      <c r="G48" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H48" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I48" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J48" s="13" t="s">
+      <c r="H48" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J48" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K48" s="12" t="s">
+      <c r="K48" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L48" s="12">
+      <c r="L48" s="10">
         <v>25</v>
       </c>
-      <c r="M48" s="14">
+      <c r="M48" s="12">
         <v>26000</v>
       </c>
-      <c r="N48" s="14">
+      <c r="N48" s="12">
         <v>650000</v>
       </c>
-      <c r="O48" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P48" s="10" t="str">
+      <c r="O48" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P48" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A49" s="11">
+      <c r="A49" s="9">
         <v>45945</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E49" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F49" s="12">
+      <c r="F49" s="10">
         <v>773750007</v>
       </c>
-      <c r="G49" s="12" t="s">
+      <c r="G49" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H49" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I49" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J49" s="13" t="s">
+      <c r="H49" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I49" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J49" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K49" s="12" t="s">
+      <c r="K49" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="L49" s="12">
+      <c r="L49" s="10">
         <v>2</v>
       </c>
-      <c r="M49" s="14">
+      <c r="M49" s="12">
         <v>15500</v>
       </c>
-      <c r="N49" s="14">
+      <c r="N49" s="12">
         <v>31000</v>
       </c>
-      <c r="O49" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P49" s="10" t="str">
+      <c r="O49" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P49" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A50" s="11">
+      <c r="A50" s="9">
         <v>45945</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C50" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E50" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F50" s="12">
+      <c r="F50" s="10">
         <v>773750007</v>
       </c>
-      <c r="G50" s="12" t="s">
+      <c r="G50" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H50" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I50" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J50" s="13" t="s">
+      <c r="H50" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I50" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J50" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K50" s="12" t="s">
+      <c r="K50" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="L50" s="12">
+      <c r="L50" s="10">
         <v>1</v>
       </c>
-      <c r="M50" s="14">
+      <c r="M50" s="12">
         <v>15500</v>
       </c>
-      <c r="N50" s="14">
+      <c r="N50" s="12">
         <v>15500</v>
       </c>
-      <c r="O50" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P50" s="10" t="str">
+      <c r="O50" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P50" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A51" s="11">
+      <c r="A51" s="9">
         <v>45945</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E51" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F51" s="12">
+      <c r="F51" s="10">
         <v>775171537</v>
       </c>
-      <c r="G51" s="12" t="s">
+      <c r="G51" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H51" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I51" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J51" s="13" t="s">
+      <c r="H51" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I51" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="K51" s="12" t="s">
+      <c r="K51" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L51" s="12">
+      <c r="L51" s="10">
         <v>25</v>
       </c>
-      <c r="M51" s="14">
+      <c r="M51" s="12">
         <v>26000</v>
       </c>
-      <c r="N51" s="14">
+      <c r="N51" s="12">
         <v>650000</v>
       </c>
-      <c r="O51" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P51" s="10" t="str">
+      <c r="O51" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P51" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A52" s="11">
+      <c r="A52" s="9">
         <v>45945</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="D52" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F52" s="12">
+      <c r="F52" s="10">
         <v>773199049</v>
       </c>
-      <c r="G52" s="12" t="s">
+      <c r="G52" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H52" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I52" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J52" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K52" s="12" t="s">
+      <c r="H52" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J52" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K52" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="L52" s="12">
+      <c r="L52" s="10">
         <v>5</v>
       </c>
-      <c r="M52" s="14">
+      <c r="M52" s="12">
         <v>10000</v>
       </c>
-      <c r="N52" s="14">
+      <c r="N52" s="12">
         <v>50000</v>
       </c>
-      <c r="O52" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P52" s="10" t="str">
+      <c r="O52" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P52" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A53" s="11">
+      <c r="A53" s="9">
         <v>45945</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E53" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F53" s="12">
+      <c r="F53" s="10">
         <v>773199049</v>
       </c>
-      <c r="G53" s="12" t="s">
+      <c r="G53" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H53" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I53" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J53" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K53" s="12" t="s">
+      <c r="H53" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J53" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K53" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="L53" s="12">
+      <c r="L53" s="10">
         <v>5</v>
       </c>
-      <c r="M53" s="14">
+      <c r="M53" s="12">
         <v>10250</v>
       </c>
-      <c r="N53" s="14">
+      <c r="N53" s="12">
         <v>51250</v>
       </c>
-      <c r="O53" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P53" s="10" t="str">
+      <c r="O53" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P53" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A54" s="11">
+      <c r="A54" s="9">
         <v>45943</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B54" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E54" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F54" s="12">
+      <c r="F54" s="10">
         <v>775661455</v>
       </c>
-      <c r="G54" s="12" t="s">
+      <c r="G54" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H54" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I54" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J54" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K54" s="12" t="s">
+      <c r="H54" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I54" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J54" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K54" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L54" s="12">
+      <c r="L54" s="10">
         <v>25</v>
       </c>
-      <c r="M54" s="14">
+      <c r="M54" s="12">
         <v>26000</v>
       </c>
-      <c r="N54" s="14">
+      <c r="N54" s="12">
         <v>650000</v>
       </c>
-      <c r="O54" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P54" s="10" t="str">
+      <c r="O54" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P54" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A55" s="11">
+      <c r="A55" s="9">
         <v>45943</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="12" t="s">
+      <c r="D55" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E55" s="12" t="s">
+      <c r="E55" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F55" s="12">
+      <c r="F55" s="10">
         <v>775661455</v>
       </c>
-      <c r="G55" s="12" t="s">
+      <c r="G55" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H55" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I55" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J55" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K55" s="12" t="s">
+      <c r="H55" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J55" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K55" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L55" s="12">
+      <c r="L55" s="10">
         <v>25</v>
       </c>
-      <c r="M55" s="14">
+      <c r="M55" s="12">
         <v>19500</v>
       </c>
-      <c r="N55" s="14">
+      <c r="N55" s="12">
         <v>487500</v>
       </c>
-      <c r="O55" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P55" s="10" t="str">
+      <c r="O55" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P55" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A56" s="11">
+      <c r="A56" s="9">
         <v>45945</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C56" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D56" s="12" t="s">
+      <c r="D56" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E56" s="12" t="s">
+      <c r="E56" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F56" s="12">
+      <c r="F56" s="10">
         <v>776818022</v>
       </c>
-      <c r="G56" s="12" t="s">
+      <c r="G56" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H56" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I56" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J56" s="13" t="s">
+      <c r="H56" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I56" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J56" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K56" s="12" t="s">
+      <c r="K56" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="L56" s="12">
+      <c r="L56" s="10">
         <v>25</v>
       </c>
-      <c r="M56" s="14">
+      <c r="M56" s="12">
         <v>9750</v>
       </c>
-      <c r="N56" s="14">
+      <c r="N56" s="12">
         <v>243750</v>
       </c>
-      <c r="O56" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P56" s="10" t="str">
+      <c r="O56" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P56" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A57" s="11">
+      <c r="A57" s="9">
         <v>45945</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C57" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D57" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E57" s="12" t="s">
+      <c r="E57" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="F57" s="12">
+      <c r="F57" s="10">
         <v>773482683</v>
       </c>
-      <c r="G57" s="12" t="s">
+      <c r="G57" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H57" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I57" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J57" s="13" t="s">
+      <c r="H57" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J57" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="K57" s="12" t="s">
+      <c r="K57" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="L57" s="12">
+      <c r="L57" s="10">
         <v>25</v>
       </c>
-      <c r="M57" s="14">
+      <c r="M57" s="12">
         <v>31000</v>
       </c>
-      <c r="N57" s="14">
+      <c r="N57" s="12">
         <v>775000</v>
       </c>
-      <c r="O57" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P57" s="10" t="str">
+      <c r="O57" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P57" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="28.15" x14ac:dyDescent="0.45">
-      <c r="A58" s="11">
+      <c r="A58" s="9">
         <v>45945</v>
       </c>
-      <c r="B58" s="12" t="s">
+      <c r="B58" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="C58" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D58" s="12" t="s">
+      <c r="D58" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E58" s="12" t="s">
+      <c r="E58" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="F58" s="12">
+      <c r="F58" s="10">
         <v>774024173</v>
       </c>
-      <c r="G58" s="12" t="s">
+      <c r="G58" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H58" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I58" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J58" s="13" t="s">
+      <c r="H58" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I58" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J58" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="K58" s="12" t="s">
+      <c r="K58" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L58" s="12">
+      <c r="L58" s="10">
         <v>50</v>
       </c>
-      <c r="M58" s="14">
+      <c r="M58" s="12">
         <v>26000</v>
       </c>
-      <c r="N58" s="14">
+      <c r="N58" s="12">
         <v>1300000</v>
       </c>
-      <c r="O58" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P58" s="10" t="str">
+      <c r="O58" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P58" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A59" s="11">
+      <c r="A59" s="9">
         <v>45945</v>
       </c>
-      <c r="B59" s="12" t="s">
+      <c r="B59" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="C59" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D59" s="12" t="s">
+      <c r="D59" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E59" s="12" t="s">
+      <c r="E59" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="F59" s="12">
+      <c r="F59" s="10">
         <v>770712599</v>
       </c>
-      <c r="G59" s="12" t="s">
+      <c r="G59" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H59" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I59" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J59" s="13" t="s">
+      <c r="H59" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I59" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J59" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="K59" s="12" t="s">
+      <c r="K59" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L59" s="12">
+      <c r="L59" s="10">
         <v>50</v>
       </c>
-      <c r="M59" s="14">
+      <c r="M59" s="12">
         <v>26000</v>
       </c>
-      <c r="N59" s="14">
+      <c r="N59" s="12">
         <v>1300000</v>
       </c>
-      <c r="O59" s="9" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S42</v>
-      </c>
-      <c r="P59" s="10" t="str">
+      <c r="O59" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S42</v>
+      </c>
+      <c r="P59" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" ht="28.15" x14ac:dyDescent="0.45">
+      <c r="A60" s="13">
+        <v>45950</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E60" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F60" s="14">
+        <v>775623289</v>
+      </c>
+      <c r="G60" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H60" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I60" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J60" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="K60" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="L60" s="14">
+        <v>5</v>
+      </c>
+      <c r="M60" s="16">
+        <v>31000</v>
+      </c>
+      <c r="N60" s="16">
+        <v>155000</v>
+      </c>
+      <c r="O60" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P60" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" ht="28.15" x14ac:dyDescent="0.45">
+      <c r="A61" s="13">
+        <v>45950</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F61" s="14">
+        <v>775623289</v>
+      </c>
+      <c r="G61" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H61" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I61" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J61" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="K61" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L61" s="14">
+        <v>2</v>
+      </c>
+      <c r="M61" s="16">
+        <v>11500</v>
+      </c>
+      <c r="N61" s="16">
+        <v>23000</v>
+      </c>
+      <c r="O61" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P61" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A62" s="13">
+        <v>45950</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="F62" s="14">
+        <v>778013213</v>
+      </c>
+      <c r="G62" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H62" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I62" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J62" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K62" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L62" s="14">
+        <v>25</v>
+      </c>
+      <c r="M62" s="16">
+        <v>19500</v>
+      </c>
+      <c r="N62" s="16">
+        <v>487500</v>
+      </c>
+      <c r="O62" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P62" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A63" s="13">
+        <v>45950</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="F63" s="14">
+        <v>778291515</v>
+      </c>
+      <c r="G63" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H63" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I63" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J63" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="K63" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="L63" s="14">
+        <v>10</v>
+      </c>
+      <c r="M63" s="16">
+        <v>31000</v>
+      </c>
+      <c r="N63" s="16">
+        <v>310000</v>
+      </c>
+      <c r="O63" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P63" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A64" s="13">
+        <v>45950</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="F64" s="14">
+        <v>772131614</v>
+      </c>
+      <c r="G64" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H64" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I64" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J64" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K64" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L64" s="14">
+        <v>6</v>
+      </c>
+      <c r="M64" s="16">
+        <v>11500</v>
+      </c>
+      <c r="N64" s="16">
+        <v>69000</v>
+      </c>
+      <c r="O64" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P64" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A65" s="13">
+        <v>45950</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F65" s="14">
+        <v>774446616</v>
+      </c>
+      <c r="G65" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="H65" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I65" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J65" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="K65" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="L65" s="14">
+        <v>1</v>
+      </c>
+      <c r="M65" s="16">
+        <v>31000</v>
+      </c>
+      <c r="N65" s="16">
+        <v>31000</v>
+      </c>
+      <c r="O65" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P65" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A66" s="13">
+        <v>45950</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="F66" s="14">
+        <v>775630094</v>
+      </c>
+      <c r="G66" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H66" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I66" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J66" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="K66" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="L66" s="14">
+        <v>15</v>
+      </c>
+      <c r="M66" s="16">
+        <v>31000</v>
+      </c>
+      <c r="N66" s="16">
+        <v>465000</v>
+      </c>
+      <c r="O66" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P66" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" ht="28.15" x14ac:dyDescent="0.45">
+      <c r="A67" s="13">
+        <v>45950</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F67" s="14">
+        <v>775623289</v>
+      </c>
+      <c r="G67" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H67" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I67" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J67" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="K67" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L67" s="14">
+        <v>20</v>
+      </c>
+      <c r="M67" s="16">
+        <v>26000</v>
+      </c>
+      <c r="N67" s="16">
+        <v>520000</v>
+      </c>
+      <c r="O67" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P67" s="18" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>

</xml_diff>

<commit_message>
Rapport du 24 Octobre 2024
</commit_message>
<xml_diff>
--- a/Donnees_RZ.xlsx
+++ b/Donnees_RZ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01447637-E130-4293-837A-45A549603C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CDF40E-592B-4FC5-99E3-8731BB65F2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10800" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semaine 1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="155">
   <si>
     <t>Date</t>
   </si>
@@ -442,6 +442,63 @@
   </si>
   <si>
     <t>Améne le reste demain stp</t>
+  </si>
+  <si>
+    <t>Pape Dieng</t>
+  </si>
+  <si>
+    <t>Lait Janus, Refraish, Meadow Cup sac 25kg</t>
+  </si>
+  <si>
+    <t>Grand Yoff</t>
+  </si>
+  <si>
+    <t>Babacar Diop</t>
+  </si>
+  <si>
+    <t>Mbacké</t>
+  </si>
+  <si>
+    <t>Client partenaire.commande reçue</t>
+  </si>
+  <si>
+    <t>Abdou Wagué</t>
+  </si>
+  <si>
+    <t>Client "partenaire". commande reçue</t>
+  </si>
+  <si>
+    <t>Ibrahima Diallo</t>
+  </si>
+  <si>
+    <t>BABACAR Cissé</t>
+  </si>
+  <si>
+    <t>Bala</t>
+  </si>
+  <si>
+    <t>Yeumbeul Mbéde Sass</t>
+  </si>
+  <si>
+    <t>NAFAR BOUTIQUE</t>
+  </si>
+  <si>
+    <t>Zone de captage</t>
+  </si>
+  <si>
+    <t>Mamadou Diallo</t>
+  </si>
+  <si>
+    <t>Bassirou NDAO</t>
+  </si>
+  <si>
+    <t>Tu as fait retarder ma commande commend</t>
+  </si>
+  <si>
+    <t>Mame Serigne</t>
+  </si>
+  <si>
+    <t>Client artenaire</t>
   </si>
 </sst>
 </file>
@@ -838,8 +895,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P67" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A1:P67" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P83" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A1:P83" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{F85C405C-E78B-4DA6-8568-08107D7551E4}" name="Date" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{24A95AD6-D6B8-4864-9451-50BFB3565C62}" name="Prenom_Nom_RZ" dataDxfId="14"/>
@@ -1152,10 +1209,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:P67"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I39" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="T64" sqref="T64"/>
+    <sheetView tabSelected="1" topLeftCell="E61" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68:N83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4244,417 +4301,1249 @@
       </c>
     </row>
     <row r="60" spans="1:16" ht="28.15" x14ac:dyDescent="0.45">
-      <c r="A60" s="13">
+      <c r="A60" s="9">
         <v>45950</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="C60" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D60" s="14" t="s">
+      <c r="D60" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E60" s="14" t="s">
+      <c r="E60" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F60" s="14">
+      <c r="F60" s="10">
         <v>775623289</v>
       </c>
-      <c r="G60" s="14" t="s">
+      <c r="G60" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H60" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I60" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J60" s="15" t="s">
+      <c r="H60" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I60" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J60" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="K60" s="14" t="s">
+      <c r="K60" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="L60" s="14">
+      <c r="L60" s="10">
         <v>5</v>
       </c>
-      <c r="M60" s="16">
+      <c r="M60" s="12">
         <v>31000</v>
       </c>
-      <c r="N60" s="16">
+      <c r="N60" s="12">
         <v>155000</v>
       </c>
-      <c r="O60" s="17" t="str">
+      <c r="O60" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S43</v>
       </c>
-      <c r="P60" s="18" t="str">
+      <c r="P60" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="61" spans="1:16" ht="28.15" x14ac:dyDescent="0.45">
-      <c r="A61" s="13">
+      <c r="A61" s="9">
         <v>45950</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="C61" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="D61" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="E61" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F61" s="14">
+      <c r="F61" s="10">
         <v>775623289</v>
       </c>
-      <c r="G61" s="14" t="s">
+      <c r="G61" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H61" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I61" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J61" s="15" t="s">
+      <c r="H61" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I61" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J61" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="K61" s="14" t="s">
+      <c r="K61" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="L61" s="14">
+      <c r="L61" s="10">
         <v>2</v>
       </c>
-      <c r="M61" s="16">
+      <c r="M61" s="12">
         <v>11500</v>
       </c>
-      <c r="N61" s="16">
+      <c r="N61" s="12">
         <v>23000</v>
       </c>
-      <c r="O61" s="17" t="str">
+      <c r="O61" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S43</v>
       </c>
-      <c r="P61" s="18" t="str">
+      <c r="P61" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A62" s="13">
+      <c r="A62" s="9">
         <v>45950</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="C62" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D62" s="14" t="s">
+      <c r="D62" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E62" s="14" t="s">
+      <c r="E62" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="F62" s="14">
+      <c r="F62" s="10">
         <v>778013213</v>
       </c>
-      <c r="G62" s="14" t="s">
+      <c r="G62" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="H62" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I62" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J62" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="K62" s="14" t="s">
+      <c r="H62" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I62" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J62" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K62" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L62" s="14">
+      <c r="L62" s="10">
         <v>25</v>
       </c>
-      <c r="M62" s="16">
+      <c r="M62" s="12">
         <v>19500</v>
       </c>
-      <c r="N62" s="16">
+      <c r="N62" s="12">
         <v>487500</v>
       </c>
-      <c r="O62" s="17" t="str">
+      <c r="O62" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S43</v>
       </c>
-      <c r="P62" s="18" t="str">
+      <c r="P62" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A63" s="13">
+      <c r="A63" s="9">
         <v>45950</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C63" s="14" t="s">
+      <c r="C63" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D63" s="14" t="s">
+      <c r="D63" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E63" s="14" t="s">
+      <c r="E63" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="F63" s="14">
+      <c r="F63" s="10">
         <v>778291515</v>
       </c>
-      <c r="G63" s="14" t="s">
+      <c r="G63" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H63" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I63" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J63" s="15" t="s">
+      <c r="H63" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I63" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J63" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K63" s="14" t="s">
+      <c r="K63" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="L63" s="14">
+      <c r="L63" s="10">
         <v>10</v>
       </c>
-      <c r="M63" s="16">
+      <c r="M63" s="12">
         <v>31000</v>
       </c>
-      <c r="N63" s="16">
+      <c r="N63" s="12">
         <v>310000</v>
       </c>
-      <c r="O63" s="17" t="str">
+      <c r="O63" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S43</v>
       </c>
-      <c r="P63" s="18" t="str">
+      <c r="P63" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A64" s="13">
+      <c r="A64" s="9">
         <v>45950</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="C64" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D64" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E64" s="14" t="s">
+      <c r="E64" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="F64" s="14">
+      <c r="F64" s="10">
         <v>772131614</v>
       </c>
-      <c r="G64" s="14" t="s">
+      <c r="G64" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H64" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I64" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J64" s="15" t="s">
+      <c r="H64" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J64" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="K64" s="14" t="s">
+      <c r="K64" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="L64" s="14">
+      <c r="L64" s="10">
         <v>6</v>
       </c>
-      <c r="M64" s="16">
+      <c r="M64" s="12">
         <v>11500</v>
       </c>
-      <c r="N64" s="16">
+      <c r="N64" s="12">
         <v>69000</v>
       </c>
-      <c r="O64" s="17" t="str">
+      <c r="O64" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S43</v>
       </c>
-      <c r="P64" s="18" t="str">
+      <c r="P64" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A65" s="13">
+      <c r="A65" s="9">
         <v>45950</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C65" s="14" t="s">
+      <c r="C65" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D65" s="14" t="s">
+      <c r="D65" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E65" s="14" t="s">
+      <c r="E65" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="F65" s="14">
+      <c r="F65" s="10">
         <v>774446616</v>
       </c>
-      <c r="G65" s="14" t="s">
+      <c r="G65" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="H65" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I65" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J65" s="15" t="s">
+      <c r="H65" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I65" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J65" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="K65" s="14" t="s">
+      <c r="K65" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="L65" s="14">
+      <c r="L65" s="10">
         <v>1</v>
       </c>
-      <c r="M65" s="16">
+      <c r="M65" s="12">
         <v>31000</v>
       </c>
-      <c r="N65" s="16">
+      <c r="N65" s="12">
         <v>31000</v>
       </c>
-      <c r="O65" s="17" t="str">
+      <c r="O65" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S43</v>
       </c>
-      <c r="P65" s="18" t="str">
+      <c r="P65" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A66" s="13">
+      <c r="A66" s="9">
         <v>45950</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C66" s="14" t="s">
+      <c r="C66" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D66" s="14" t="s">
+      <c r="D66" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E66" s="14" t="s">
+      <c r="E66" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="F66" s="14">
+      <c r="F66" s="10">
         <v>775630094</v>
       </c>
-      <c r="G66" s="14" t="s">
+      <c r="G66" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H66" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I66" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J66" s="15" t="s">
+      <c r="H66" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J66" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="K66" s="14" t="s">
+      <c r="K66" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="L66" s="14">
+      <c r="L66" s="10">
         <v>15</v>
       </c>
-      <c r="M66" s="16">
+      <c r="M66" s="12">
         <v>31000</v>
       </c>
-      <c r="N66" s="16">
+      <c r="N66" s="12">
         <v>465000</v>
       </c>
-      <c r="O66" s="17" t="str">
+      <c r="O66" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S43</v>
       </c>
-      <c r="P66" s="18" t="str">
+      <c r="P66" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>
     </row>
     <row r="67" spans="1:16" ht="28.15" x14ac:dyDescent="0.45">
-      <c r="A67" s="13">
+      <c r="A67" s="9">
         <v>45950</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C67" s="14" t="s">
+      <c r="C67" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D67" s="14" t="s">
+      <c r="D67" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E67" s="14" t="s">
+      <c r="E67" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F67" s="14">
+      <c r="F67" s="10">
         <v>775623289</v>
       </c>
-      <c r="G67" s="14" t="s">
+      <c r="G67" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H67" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I67" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J67" s="15" t="s">
+      <c r="H67" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J67" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="K67" s="14" t="s">
+      <c r="K67" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L67" s="14">
+      <c r="L67" s="10">
         <v>20</v>
       </c>
-      <c r="M67" s="16">
+      <c r="M67" s="12">
         <v>26000</v>
       </c>
-      <c r="N67" s="16">
+      <c r="N67" s="12">
         <v>520000</v>
       </c>
-      <c r="O67" s="17" t="str">
+      <c r="O67" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S43</v>
       </c>
-      <c r="P67" s="18" t="str">
+      <c r="P67" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A68" s="13">
+        <v>45953</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F68" s="14">
+        <v>778096419</v>
+      </c>
+      <c r="G68" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H68" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I68" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J68" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="K68" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="L68" s="14">
+        <v>5</v>
+      </c>
+      <c r="M68" s="16">
+        <v>60000</v>
+      </c>
+      <c r="N68" s="16">
+        <v>300000</v>
+      </c>
+      <c r="O68" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P68" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A69" s="13">
+        <v>45953</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="F69" s="14">
+        <v>774880562</v>
+      </c>
+      <c r="G69" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H69" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I69" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J69" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K69" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L69" s="14">
+        <v>50</v>
+      </c>
+      <c r="M69" s="16">
+        <v>26000</v>
+      </c>
+      <c r="N69" s="16">
+        <v>1300000</v>
+      </c>
+      <c r="O69" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P69" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A70" s="13">
+        <v>45953</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="F70" s="14">
+        <v>779486095</v>
+      </c>
+      <c r="G70" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H70" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I70" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J70" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="K70" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="L70" s="14">
+        <v>25</v>
+      </c>
+      <c r="M70" s="16">
+        <v>12500</v>
+      </c>
+      <c r="N70" s="16">
+        <v>312500</v>
+      </c>
+      <c r="O70" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P70" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A71" s="13">
+        <v>45953</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F71" s="14">
+        <v>764970202</v>
+      </c>
+      <c r="G71" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H71" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I71" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J71" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="K71" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L71" s="14">
+        <v>10</v>
+      </c>
+      <c r="M71" s="16">
+        <v>15500</v>
+      </c>
+      <c r="N71" s="16">
+        <v>155000</v>
+      </c>
+      <c r="O71" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P71" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A72" s="13">
+        <v>45953</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F72" s="14">
+        <v>764970202</v>
+      </c>
+      <c r="G72" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H72" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I72" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J72" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="K72" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="L72" s="14">
+        <v>15</v>
+      </c>
+      <c r="M72" s="16">
+        <v>15500</v>
+      </c>
+      <c r="N72" s="16">
+        <v>232500</v>
+      </c>
+      <c r="O72" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P72" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A73" s="13">
+        <v>45952</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="F73" s="14">
+        <v>775784714</v>
+      </c>
+      <c r="G73" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H73" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I73" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J73" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K73" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L73" s="14">
+        <v>5</v>
+      </c>
+      <c r="M73" s="16">
+        <v>11500</v>
+      </c>
+      <c r="N73" s="16">
+        <v>57500</v>
+      </c>
+      <c r="O73" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P73" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A74" s="13">
+        <v>45952</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F74" s="14">
+        <v>783682649</v>
+      </c>
+      <c r="G74" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H74" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I74" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J74" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="K74" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L74" s="14">
+        <v>300</v>
+      </c>
+      <c r="M74" s="16">
+        <v>6000</v>
+      </c>
+      <c r="N74" s="16">
+        <v>1800000</v>
+      </c>
+      <c r="O74" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P74" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A75" s="13">
+        <v>45952</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F75" s="14">
+        <v>776175166</v>
+      </c>
+      <c r="G75" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H75" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I75" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J75" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="K75" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L75" s="14">
+        <v>100</v>
+      </c>
+      <c r="M75" s="16">
+        <v>26000</v>
+      </c>
+      <c r="N75" s="16">
+        <v>2600000</v>
+      </c>
+      <c r="O75" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P75" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A76" s="13">
+        <v>45952</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E76" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F76" s="14">
+        <v>783682649</v>
+      </c>
+      <c r="G76" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H76" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I76" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="K76" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L76" s="14">
+        <v>5</v>
+      </c>
+      <c r="M76" s="16">
+        <v>11500</v>
+      </c>
+      <c r="N76" s="16">
+        <v>57500</v>
+      </c>
+      <c r="O76" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P76" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A77" s="13">
+        <v>45952</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E77" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="F77" s="14">
+        <v>762974040</v>
+      </c>
+      <c r="G77" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H77" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I77" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J77" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K77" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L77" s="14">
+        <v>25</v>
+      </c>
+      <c r="M77" s="16">
+        <v>26000</v>
+      </c>
+      <c r="N77" s="16">
+        <v>650000</v>
+      </c>
+      <c r="O77" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P77" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A78" s="13">
+        <v>45952</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E78" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F78" s="14">
+        <v>781681995</v>
+      </c>
+      <c r="G78" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H78" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I78" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J78" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K78" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="L78" s="14">
+        <v>1</v>
+      </c>
+      <c r="M78" s="16">
+        <v>12500</v>
+      </c>
+      <c r="N78" s="16">
+        <v>12500</v>
+      </c>
+      <c r="O78" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P78" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A79" s="13">
+        <v>45952</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="F79" s="14">
+        <v>775630094</v>
+      </c>
+      <c r="G79" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H79" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I79" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J79" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K79" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="L79" s="14">
+        <v>11</v>
+      </c>
+      <c r="M79" s="16">
+        <v>31000</v>
+      </c>
+      <c r="N79" s="16">
+        <v>341000</v>
+      </c>
+      <c r="O79" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P79" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A80" s="13">
+        <v>45952</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E80" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F80" s="14">
+        <v>775544532</v>
+      </c>
+      <c r="G80" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H80" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I80" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J80" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="K80" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L80" s="14">
+        <v>25</v>
+      </c>
+      <c r="M80" s="16">
+        <v>26000</v>
+      </c>
+      <c r="N80" s="16">
+        <v>650000</v>
+      </c>
+      <c r="O80" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P80" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A81" s="13">
+        <v>45952</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E81" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F81" s="14">
+        <v>777772248</v>
+      </c>
+      <c r="G81" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H81" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I81" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J81" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="K81" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L81" s="14">
+        <v>5</v>
+      </c>
+      <c r="M81" s="16">
+        <v>11500</v>
+      </c>
+      <c r="N81" s="16">
+        <v>57500</v>
+      </c>
+      <c r="O81" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P81" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A82" s="13">
+        <v>45952</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E82" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F82" s="14">
+        <v>775538380</v>
+      </c>
+      <c r="G82" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H82" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="I82" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J82" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="K82" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L82" s="14">
+        <v>1</v>
+      </c>
+      <c r="M82" s="16">
+        <v>19500</v>
+      </c>
+      <c r="N82" s="16">
+        <v>19500</v>
+      </c>
+      <c r="O82" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P82" s="18" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>octobre</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A83" s="13">
+        <v>45952</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F83" s="14">
+        <v>770571683</v>
+      </c>
+      <c r="G83" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H83" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I83" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J83" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="K83" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="L83" s="14">
+        <v>1</v>
+      </c>
+      <c r="M83" s="16">
+        <v>15500</v>
+      </c>
+      <c r="N83" s="16">
+        <v>15500</v>
+      </c>
+      <c r="O83" s="17" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S43</v>
+      </c>
+      <c r="P83" s="18" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>octobre</v>
       </c>

</xml_diff>

<commit_message>
Rapport du 07 Novembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_RZ.xlsx
+++ b/Donnees_RZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFE7227-84C2-430B-B762-427BD064DD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E82D60-D003-46E7-83C4-52141C0B8A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10800" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -210,6 +210,51 @@
   </si>
   <si>
     <t>Jus Lido</t>
+  </si>
+  <si>
+    <t>NAFAR BOUTIQUE</t>
+  </si>
+  <si>
+    <t>Café pot Refraish 200g</t>
+  </si>
+  <si>
+    <t>Marché Bou Bess</t>
+  </si>
+  <si>
+    <t>MOUSTAPHA BAKHDAD</t>
+  </si>
+  <si>
+    <t>Grand Yoff</t>
+  </si>
+  <si>
+    <t>Abdou Diallo</t>
+  </si>
+  <si>
+    <t>Fatoumata TRAORE</t>
+  </si>
+  <si>
+    <t>KEUR MASSAR</t>
+  </si>
+  <si>
+    <t>Terminus 54</t>
+  </si>
+  <si>
+    <t>BABACAR Cissé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAS </t>
+  </si>
+  <si>
+    <t>Keur Massar Ainoumady</t>
+  </si>
+  <si>
+    <t>Pape</t>
+  </si>
+  <si>
+    <t>Demi-Gros</t>
+  </si>
+  <si>
+    <t>Raa</t>
   </si>
 </sst>
 </file>
@@ -277,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -298,6 +343,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -313,6 +364,25 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -353,30 +423,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-        <name val="TIMES"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -403,6 +449,7 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -529,27 +576,31 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color auto="1"/>
+        <name val="TIMES"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -599,10 +650,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P15" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="16" tableBorderDxfId="17">
-  <autoFilter ref="A1:P15" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P20" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A1:P20" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{F85C405C-E78B-4DA6-8568-08107D7551E4}" name="Date" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{F85C405C-E78B-4DA6-8568-08107D7551E4}" name="Date" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{24A95AD6-D6B8-4864-9451-50BFB3565C62}" name="Prenom_Nom_RZ" dataDxfId="14"/>
     <tableColumn id="4" xr3:uid="{72E50CE0-52B1-4C49-9D23-C97154D649A5}" name="zone" dataDxfId="13"/>
     <tableColumn id="5" xr3:uid="{E26577ED-9647-48EE-BE53-9D2F344CB36B}" name="secteur" dataDxfId="12"/>
@@ -611,15 +662,15 @@
     <tableColumn id="8" xr3:uid="{8D4D921E-310A-44FC-AA1D-F30B627C5984}" name="Type" dataDxfId="9"/>
     <tableColumn id="10" xr3:uid="{636AF8A9-C9D0-49B6-94C8-FFB87B44FA47}" name="Point_de_Vente" dataDxfId="8"/>
     <tableColumn id="11" xr3:uid="{35E41B20-D7EB-4025-A9CC-62B85956ABCD}" name="Operation" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{AB905DE1-CC5E-4C11-8318-9C04B6D96EC3}" name="Commentaire" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{9BC88C3B-EEBD-4156-81CB-075746F3F057}" name="Produit" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{8DD706C4-BCF7-47C0-9913-F482F7A2F321}" name="Quantites" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{D96EE09E-B22B-4D75-AABE-AEBF7CE286A6}" name="Prix_Unitaire" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{B1727D51-96B6-4015-83C5-EBCAD96E9834}" name="Prix Total" dataDxfId="0"/>
-    <tableColumn id="17" xr3:uid="{9A2C6D78-CE06-4E13-B8E1-0CB92B201156}" name="Semaine" dataDxfId="15">
+    <tableColumn id="12" xr3:uid="{AB905DE1-CC5E-4C11-8318-9C04B6D96EC3}" name="Commentaire" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{9BC88C3B-EEBD-4156-81CB-075746F3F057}" name="Produit" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{8DD706C4-BCF7-47C0-9913-F482F7A2F321}" name="Quantites" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{D96EE09E-B22B-4D75-AABE-AEBF7CE286A6}" name="Prix_Unitaire" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{B1727D51-96B6-4015-83C5-EBCAD96E9834}" name="Prix Total" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{9A2C6D78-CE06-4E13-B8E1-0CB92B201156}" name="Semaine" dataDxfId="1">
       <calculatedColumnFormula>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{83F3E9A5-7911-47C6-B543-07173CE7D4B5}" name="Mois" dataDxfId="4">
+    <tableColumn id="18" xr3:uid="{83F3E9A5-7911-47C6-B543-07173CE7D4B5}" name="Mois" dataDxfId="0">
       <calculatedColumnFormula>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -913,10 +964,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A16" sqref="A16:N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1031,11 +1082,11 @@
       <c r="N2" s="11">
         <v>650000</v>
       </c>
-      <c r="O2" s="12" t="str">
+      <c r="O2" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S45</v>
       </c>
-      <c r="P2" s="13" t="str">
+      <c r="P2" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1083,11 +1134,11 @@
       <c r="N3" s="11">
         <v>650000</v>
       </c>
-      <c r="O3" s="12" t="str">
+      <c r="O3" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S45</v>
       </c>
-      <c r="P3" s="13" t="str">
+      <c r="P3" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1135,11 +1186,11 @@
       <c r="N4" s="11">
         <v>19500</v>
       </c>
-      <c r="O4" s="12" t="str">
+      <c r="O4" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S45</v>
       </c>
-      <c r="P4" s="13" t="str">
+      <c r="P4" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1187,11 +1238,11 @@
       <c r="N5" s="11">
         <v>650000</v>
       </c>
-      <c r="O5" s="12" t="str">
+      <c r="O5" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S45</v>
       </c>
-      <c r="P5" s="13" t="str">
+      <c r="P5" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1239,11 +1290,11 @@
       <c r="N6" s="11">
         <v>150000</v>
       </c>
-      <c r="O6" s="12" t="str">
+      <c r="O6" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S45</v>
       </c>
-      <c r="P6" s="13" t="str">
+      <c r="P6" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1291,11 +1342,11 @@
       <c r="N7" s="11">
         <v>15500</v>
       </c>
-      <c r="O7" s="12" t="str">
+      <c r="O7" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S45</v>
       </c>
-      <c r="P7" s="13" t="str">
+      <c r="P7" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1343,11 +1394,11 @@
       <c r="N8" s="11">
         <v>1675000</v>
       </c>
-      <c r="O8" s="12" t="str">
+      <c r="O8" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S45</v>
       </c>
-      <c r="P8" s="13" t="str">
+      <c r="P8" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1395,11 +1446,11 @@
       <c r="N9" s="11">
         <v>650000</v>
       </c>
-      <c r="O9" s="12" t="str">
+      <c r="O9" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S45</v>
       </c>
-      <c r="P9" s="13" t="str">
+      <c r="P9" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1447,11 +1498,11 @@
       <c r="N10" s="11">
         <v>650000</v>
       </c>
-      <c r="O10" s="12" t="str">
+      <c r="O10" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S45</v>
       </c>
-      <c r="P10" s="13" t="str">
+      <c r="P10" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1499,11 +1550,11 @@
       <c r="N11" s="11">
         <v>312500</v>
       </c>
-      <c r="O11" s="12" t="str">
+      <c r="O11" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S45</v>
       </c>
-      <c r="P11" s="13" t="str">
+      <c r="P11" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1551,11 +1602,11 @@
       <c r="N12" s="11">
         <v>67000</v>
       </c>
-      <c r="O12" s="12" t="str">
+      <c r="O12" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S45</v>
       </c>
-      <c r="P12" s="13" t="str">
+      <c r="P12" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1603,11 +1654,11 @@
       <c r="N13" s="11">
         <v>62000</v>
       </c>
-      <c r="O13" s="12" t="str">
+      <c r="O13" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S45</v>
       </c>
-      <c r="P13" s="13" t="str">
+      <c r="P13" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1655,11 +1706,11 @@
       <c r="N14" s="11">
         <v>24000</v>
       </c>
-      <c r="O14" s="12" t="str">
+      <c r="O14" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S45</v>
       </c>
-      <c r="P14" s="13" t="str">
+      <c r="P14" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1707,11 +1758,271 @@
       <c r="N15" s="11">
         <v>67000</v>
       </c>
-      <c r="O15" s="12" t="str">
+      <c r="O15" s="7" t="str">
         <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
         <v>S45</v>
       </c>
-      <c r="P15" s="13" t="str">
+      <c r="P15" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>novembre</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A16" s="12">
+        <v>45968</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="13">
+        <v>762974040</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" s="13">
+        <v>10</v>
+      </c>
+      <c r="M16" s="15">
+        <v>19500</v>
+      </c>
+      <c r="N16" s="15">
+        <v>195000</v>
+      </c>
+      <c r="O16" s="16" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S45</v>
+      </c>
+      <c r="P16" s="17" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>novembre</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A17" s="12">
+        <v>45968</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="13">
+        <v>776180875</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="L17" s="13">
+        <v>15</v>
+      </c>
+      <c r="M17" s="15">
+        <v>19500</v>
+      </c>
+      <c r="N17" s="15">
+        <v>292500</v>
+      </c>
+      <c r="O17" s="16" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S45</v>
+      </c>
+      <c r="P17" s="17" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>novembre</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A18" s="12">
+        <v>45967</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="13">
+        <v>775250570</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L18" s="13">
+        <v>25</v>
+      </c>
+      <c r="M18" s="15">
+        <v>9750</v>
+      </c>
+      <c r="N18" s="15">
+        <v>243750</v>
+      </c>
+      <c r="O18" s="16" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S45</v>
+      </c>
+      <c r="P18" s="17" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>novembre</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A19" s="12">
+        <v>45967</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="13">
+        <v>783682649</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" s="13">
+        <v>25</v>
+      </c>
+      <c r="M19" s="15">
+        <v>9750</v>
+      </c>
+      <c r="N19" s="15">
+        <v>243750</v>
+      </c>
+      <c r="O19" s="16" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S45</v>
+      </c>
+      <c r="P19" s="17" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>novembre</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A20" s="12">
+        <v>45967</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="13">
+        <v>785107921</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="13">
+        <v>25</v>
+      </c>
+      <c r="M20" s="15">
+        <v>26000</v>
+      </c>
+      <c r="N20" s="15">
+        <v>650000</v>
+      </c>
+      <c r="O20" s="16" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S45</v>
+      </c>
+      <c r="P20" s="17" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>

</xml_diff>

<commit_message>
Rapport du 22 Novembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_RZ.xlsx
+++ b/Donnees_RZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FECEE6-76C8-43B4-9550-4AA845E93F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E226FB70-4C54-48F2-93AE-D8CEA2FE9DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="277" yWindow="37" windowWidth="18923" windowHeight="10763" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="92">
   <si>
     <t>Date</t>
   </si>
@@ -297,6 +297,18 @@
   </si>
   <si>
     <t>Wane</t>
+  </si>
+  <si>
+    <t>Ndack NDAO</t>
+  </si>
+  <si>
+    <t>GUEDIAWAYE</t>
+  </si>
+  <si>
+    <t>Yeumbeul Mbéde Sass</t>
+  </si>
+  <si>
+    <t>MAMDOU DIA</t>
   </si>
 </sst>
 </file>
@@ -364,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -385,6 +397,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -686,8 +704,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P28" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A1:P28" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P30" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A1:P30" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{F85C405C-E78B-4DA6-8568-08107D7551E4}" name="Date" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{24A95AD6-D6B8-4864-9451-50BFB3565C62}" name="Prenom_Nom_RZ" dataDxfId="14"/>
@@ -1000,10 +1018,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="G23" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1118,11 +1136,11 @@
       <c r="N2" s="11">
         <v>243750</v>
       </c>
-      <c r="O2" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P2" s="13" t="str">
+      <c r="O2" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P2" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1170,11 +1188,11 @@
       <c r="N3" s="11">
         <v>97500</v>
       </c>
-      <c r="O3" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P3" s="13" t="str">
+      <c r="O3" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P3" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1222,11 +1240,11 @@
       <c r="N4" s="11">
         <v>46500</v>
       </c>
-      <c r="O4" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P4" s="13" t="str">
+      <c r="O4" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P4" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1274,11 +1292,11 @@
       <c r="N5" s="11">
         <v>46500</v>
       </c>
-      <c r="O5" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P5" s="13" t="str">
+      <c r="O5" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P5" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1326,11 +1344,11 @@
       <c r="N6" s="11">
         <v>12500</v>
       </c>
-      <c r="O6" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P6" s="13" t="str">
+      <c r="O6" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P6" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1378,11 +1396,11 @@
       <c r="N7" s="11">
         <v>10000</v>
       </c>
-      <c r="O7" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P7" s="13" t="str">
+      <c r="O7" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P7" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1430,11 +1448,11 @@
       <c r="N8" s="11">
         <v>487500</v>
       </c>
-      <c r="O8" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P8" s="13" t="str">
+      <c r="O8" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P8" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1482,11 +1500,11 @@
       <c r="N9" s="11">
         <v>9750</v>
       </c>
-      <c r="O9" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P9" s="13" t="str">
+      <c r="O9" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P9" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1534,11 +1552,11 @@
       <c r="N10" s="11">
         <v>23000</v>
       </c>
-      <c r="O10" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P10" s="13" t="str">
+      <c r="O10" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P10" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1586,11 +1604,11 @@
       <c r="N11" s="11">
         <v>9750</v>
       </c>
-      <c r="O11" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P11" s="13" t="str">
+      <c r="O11" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P11" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1638,11 +1656,11 @@
       <c r="N12" s="11">
         <v>75000</v>
       </c>
-      <c r="O12" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P12" s="13" t="str">
+      <c r="O12" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P12" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1690,11 +1708,11 @@
       <c r="N13" s="11">
         <v>180000</v>
       </c>
-      <c r="O13" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P13" s="13" t="str">
+      <c r="O13" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P13" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1742,11 +1760,11 @@
       <c r="N14" s="11">
         <v>1500000</v>
       </c>
-      <c r="O14" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P14" s="13" t="str">
+      <c r="O14" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P14" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1794,11 +1812,11 @@
       <c r="N15" s="11">
         <v>243750</v>
       </c>
-      <c r="O15" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P15" s="13" t="str">
+      <c r="O15" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P15" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1846,11 +1864,11 @@
       <c r="N16" s="11">
         <v>650000</v>
       </c>
-      <c r="O16" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P16" s="13" t="str">
+      <c r="O16" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P16" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1898,11 +1916,11 @@
       <c r="N17" s="11">
         <v>650000</v>
       </c>
-      <c r="O17" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P17" s="13" t="str">
+      <c r="O17" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P17" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -1950,11 +1968,11 @@
       <c r="N18" s="11">
         <v>390000</v>
       </c>
-      <c r="O18" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P18" s="13" t="str">
+      <c r="O18" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P18" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -2002,11 +2020,11 @@
       <c r="N19" s="11">
         <v>1300000</v>
       </c>
-      <c r="O19" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P19" s="13" t="str">
+      <c r="O19" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P19" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -2054,11 +2072,11 @@
       <c r="N20" s="11">
         <v>1300000</v>
       </c>
-      <c r="O20" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P20" s="13" t="str">
+      <c r="O20" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P20" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -2106,11 +2124,11 @@
       <c r="N21" s="11">
         <v>650000</v>
       </c>
-      <c r="O21" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P21" s="13" t="str">
+      <c r="O21" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P21" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -2158,11 +2176,11 @@
       <c r="N22" s="11">
         <v>650000</v>
       </c>
-      <c r="O22" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P22" s="13" t="str">
+      <c r="O22" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P22" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -2210,11 +2228,11 @@
       <c r="N23" s="11">
         <v>650000</v>
       </c>
-      <c r="O23" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P23" s="13" t="str">
+      <c r="O23" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P23" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -2262,11 +2280,11 @@
       <c r="N24" s="11">
         <v>62500</v>
       </c>
-      <c r="O24" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P24" s="13" t="str">
+      <c r="O24" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P24" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -2314,11 +2332,11 @@
       <c r="N25" s="11">
         <v>387500</v>
       </c>
-      <c r="O25" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P25" s="13" t="str">
+      <c r="O25" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P25" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -2366,11 +2384,11 @@
       <c r="N26" s="11">
         <v>77500</v>
       </c>
-      <c r="O26" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P26" s="13" t="str">
+      <c r="O26" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P26" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -2418,11 +2436,11 @@
       <c r="N27" s="11">
         <v>312500</v>
       </c>
-      <c r="O27" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P27" s="13" t="str">
+      <c r="O27" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P27" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>
@@ -2470,11 +2488,115 @@
       <c r="N28" s="11">
         <v>243750</v>
       </c>
-      <c r="O28" s="12" t="str">
-        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
-        <v>S47</v>
-      </c>
-      <c r="P28" s="13" t="str">
+      <c r="O28" s="7" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P28" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>novembre</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A29" s="12">
+        <v>45983</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" s="13">
+        <v>768059355</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L29" s="13">
+        <v>50</v>
+      </c>
+      <c r="M29" s="15">
+        <v>30000</v>
+      </c>
+      <c r="N29" s="15">
+        <v>1500000</v>
+      </c>
+      <c r="O29" s="16" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P29" s="17" t="str">
+        <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
+        <v>novembre</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A30" s="12">
+        <v>45983</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" s="13">
+        <v>768059355</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30" s="13">
+        <v>50</v>
+      </c>
+      <c r="M30" s="15">
+        <v>30000</v>
+      </c>
+      <c r="N30" s="15">
+        <v>1500000</v>
+      </c>
+      <c r="O30" s="16" t="str">
+        <f>"S"&amp;_xlfn.ISOWEEKNUM(Semaine_1[[#This Row],[Date]])</f>
+        <v>S47</v>
+      </c>
+      <c r="P30" s="17" t="str">
         <f>TEXT(Semaine_1[[#This Row],[Date]],"MMMM")</f>
         <v>novembre</v>
       </c>

</xml_diff>

<commit_message>
Rapport du 01 Decembre 2025
</commit_message>
<xml_diff>
--- a/Donnees_RZ.xlsx
+++ b/Donnees_RZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NDAO ABDOULAYE\Desktop\AFRIKA LEYRI\Rapport\Promoteur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654ED5B5-928C-423C-B216-4FF75356991F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6DBC40-A445-49F6-A6EF-4EE863FC2121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" tabRatio="470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -786,9 +786,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}" name="Semaine_1" displayName="Semaine_1" ref="A1:P54" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="A1:P54" xr:uid="{FC757211-1341-459A-BE29-FAC5D7146FA5}">
-    <filterColumn colId="1">
+    <filterColumn colId="14">
       <filters>
-        <filter val="Seynabou SOW"/>
+        <filter val="S48"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1106,8 +1106,8 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="E33" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1491,7 +1491,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A8" s="8">
         <v>45979</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A9" s="8">
         <v>45979</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A10" s="8">
         <v>45979</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" s="8">
         <v>45979</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" s="8">
         <v>45980</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A32" s="8">
         <v>45985</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A33" s="8">
         <v>45985</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A34" s="8">
         <v>45985</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A37" s="8">
         <v>45986</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A38" s="8">
         <v>45986</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A39" s="8">
         <v>45986</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A40" s="8">
         <v>45986</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A41" s="8">
         <v>45986</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A42" s="8">
         <v>45986</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A43" s="8">
         <v>45986</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A44" s="8">
         <v>45986</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A45" s="8">
         <v>45986</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A46" s="8">
         <v>45991</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A47" s="8">
         <v>45991</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A48" s="8">
         <v>45990</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A49" s="8">
         <v>45990</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A50" s="8">
         <v>45990</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A51" s="8">
         <v>45989</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A52" s="8">
         <v>45989</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A53" s="8">
         <v>45988</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>novembre</v>
       </c>
     </row>
-    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A54" s="8">
         <v>45987</v>
       </c>

</xml_diff>